<commit_message>
Validacion actualizada con correcciones de modelos y demas, basicamente se hizo una traduccion de los requisitos del experto, se ejecuto para RQ1 Y RQ2 BERT-Score y para RQ4 Y RQ5 se quito la similitud
</commit_message>
<xml_diff>
--- a/validacion/SALIDARQ1_EXPERTO.xlsx
+++ b/validacion/SALIDARQ1_EXPERTO.xlsx
@@ -40,7 +40,7 @@
     <t xml:space="preserve">SEC-CAT-BAC-001</t>
   </si>
   <si>
-    <t xml:space="preserve">The application will implement and apply dual access control prior to deleting users, medical records.</t>
+    <t xml:space="preserve">La aplicación implementará y aplicará un doble control de acceso antes de eliminar usuarios, historiales médicos. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-53 Rev.5 AC-3, HIPAA 45 CFR §164.312(a)(1), ISO/IEC 27002:2022 5.15</t>
@@ -55,7 +55,7 @@
     <t xml:space="preserve">SEC-CAT-BAC-002</t>
   </si>
   <si>
-    <t xml:space="preserve">The application must incorporate robust access control mechanisms to prevent circumvention of access control checks by manipulating the URL.</t>
+    <t xml:space="preserve">La aplicación debe incorporar mecanismos robustos de control de acceso para evitar la elusión de las comprobaciones de control de acceso mediante la manipulación de la URL. Deben evitarse y contrarrestarse las siguientes tácticas de elusión del control de acceso: 1. Modificación de la URL (manipulación de parámetros o navegación forzada). 2. Modificación del estado interno de la aplicación. 3. Modificación de la página HTML. 4. Uso de herramientas de ataque para modificar las peticiones API </t>
   </si>
   <si>
     <t xml:space="preserve">OWASP A01:2021, CWE-639, NIST SP 800-53 AC-4, AC-6(1)</t>
@@ -67,7 +67,7 @@
     <t xml:space="preserve">SEC-CAT-BAC-003</t>
   </si>
   <si>
-    <t xml:space="preserve">The application must implement security measures to prevent the elevation of privileges.</t>
+    <t xml:space="preserve">La aplicación debe implementar medidas de seguridad para prevenir la elevación de privilegios. Evitar situaciones en las que un usuario pueda actuar sin estar autenticado o un administrador pueda actuar como un usuario normal después de iniciar sesión. </t>
   </si>
   <si>
     <t xml:space="preserve">OWASP A01:2021, NIST SP 800-53 AC-2(4), ISO/IEC 27002:2022 5.18</t>
@@ -79,7 +79,7 @@
     <t xml:space="preserve">SEC-CAT-BAC-004</t>
   </si>
   <si>
-    <t xml:space="preserve">The application must enforce strict and flexible access controls for authorized users, preventing unauthorized access to the API.</t>
+    <t xml:space="preserve">La aplicación debe aplicar controles de acceso estrictos y flexibles para los usuarios autorizados, impidiendo el acceso no autorizado a la API y garantizando la propiedad de los registros. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-53 AC-3, AC-6, ISO/IEC 27002:2022 5.17</t>
@@ -91,7 +91,7 @@
     <t xml:space="preserve">SEC-CAT-BAC-005</t>
   </si>
   <si>
-    <t xml:space="preserve">The application must prevent unauthorized access to data processing devices and assign roles to protect ePHI.</t>
+    <t xml:space="preserve">La aplicación debe impedir el acceso no autorizado a los dispositivos de procesamiento de datos y asignar funciones a los usuarios para proteger la integridad de la ePHI frente a alteraciones no autorizadas. </t>
   </si>
   <si>
     <t xml:space="preserve">HIPAA §164.312(a)(1), NIST SP 800-53 AC-2, AC-19</t>
@@ -103,7 +103,7 @@
     <t xml:space="preserve">SEC-CAT-BAC-006</t>
   </si>
   <si>
-    <t xml:space="preserve">The system must allow users to be assigned to workgroups and grant access based on these groups.</t>
+    <t xml:space="preserve">El sistema debe permitir la asignación de usuarios a grupos de trabajo y conceder acceso a los registros en función de estos grupos. Este acceso puede ser a través de una estación de trabajo, transacción, programa, proceso u otro mecanismo. </t>
   </si>
   <si>
     <t xml:space="preserve">ISO/IEC 27002:2022 5.18, NIST SP 800-53 AC-2(7), SIREN</t>
@@ -115,7 +115,7 @@
     <t xml:space="preserve">SEC-CAT-BAC-007</t>
   </si>
   <si>
-    <t xml:space="preserve">The system must implement measures to control who uses the system by authenticating with individual and then group authenticators.</t>
+    <t xml:space="preserve">El sistema debe aplicar medidas para controlar quién utiliza el sistema de tratamiento de datos, garantizando que los usuarios se autentiquen con un autentificador individual antes de utilizar un autentificador de grupo. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-53 IA-2, IA-8, ISO/IEC 27002:2022 5.15</t>
@@ -127,7 +127,7 @@
     <t xml:space="preserve">SEC-CAT-BAC-008</t>
   </si>
   <si>
-    <t xml:space="preserve">The system is required to establish a formal process for user registration and deregistration.</t>
+    <t xml:space="preserve">El sistema debe establecer un proceso formal de alta y baja de usuarios que facilite el acceso a los sistemas de información sanitaria. Este proceso debe garantizar un alineamiento consistente entre el nivel de autenticación, el mapeo de usuarios a roles, roles a funciones del sistema, y el nivel de acceso a ser otorgado al usuario. </t>
   </si>
   <si>
     <t xml:space="preserve">ISO/IEC 27002:2022 5.17, NIST SP 800-53 AC-2, SIREN</t>
@@ -139,7 +139,7 @@
     <t xml:space="preserve">SEC-CAT-CRF-001</t>
   </si>
   <si>
-    <t xml:space="preserve">The system must implement a robust FIPS-validated cryptographic infrastructure.</t>
+    <t xml:space="preserve">El sistema debe implantar una infraestructura criptográfica robusta validada por FIPS para cifrar y descifrar la información sanitaria protegida electrónicamente con el fin de garantizar una protección adecuada de la información sensible. </t>
   </si>
   <si>
     <t xml:space="preserve">HIPAA §164.312(e)(1), FIPS 140-2, NIST SP 800-53 SC-12</t>
@@ -151,7 +151,7 @@
     <t xml:space="preserve">SEC-CAT-CRF-002</t>
   </si>
   <si>
-    <t xml:space="preserve">The application must ensure security of ePHI during transmission.</t>
+    <t xml:space="preserve">La aplicación debe garantizar la seguridad de la integridad y confidencialidad durante la transmisión de la ePHI a través de redes electrónicas siguiendo las normas de salvaguarda técnica establecidas en el marco normativo. </t>
   </si>
   <si>
     <t xml:space="preserve">HIPAA §164.312(e)(1), NIST SP 800-53 SC-12, SC-13</t>
@@ -163,7 +163,7 @@
     <t xml:space="preserve">SEC-CAT-CRF-003</t>
   </si>
   <si>
-    <t xml:space="preserve">The application must ensure secure storage of the session identifier, ensuring that at no time is the generated session ID included in requests via the URL.</t>
+    <t xml:space="preserve">La aplicación debe garantizar el almacenamiento seguro del identificador de sesión, asegurando que en ningún momento se incluya el identificador de sesión generado en las peticiones a través de la URL. </t>
   </si>
   <si>
     <t xml:space="preserve">OWASP A07:2021, NIST SP 800-53 SC-23, ISO/IEC 27002:2022 8.26</t>
@@ -175,7 +175,7 @@
     <t xml:space="preserve">SEC-CAT-CRF-004</t>
   </si>
   <si>
-    <t xml:space="preserve">The application must ensure message encryption when the SessionIndex is linked to privacy data.</t>
+    <t xml:space="preserve">La aplicación debe garantizar el cifrado de los mensajes cuando el SessionIndex esté vinculado a datos de privacidad. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-53 SC-12, SC-13, ISO/IEC 27002:2022 10.1</t>
@@ -187,7 +187,7 @@
     <t xml:space="preserve">SEC-CAT-CRF-005</t>
   </si>
   <si>
-    <t xml:space="preserve">The application must exclusively store cryptographic representations of passwords, following best practices and using FIPS-validated cryptographic modules.</t>
+    <t xml:space="preserve">La aplicación debe almacenar exclusivamente representaciones criptográficas de contraseñas, siguiendo las mejores prácticas y utilizando módulos criptográficos validados por FIPS. </t>
   </si>
   <si>
     <t xml:space="preserve">HIPAA §164.312(d), NIST SP 800-53 IA-5(1), FIPS 140-2</t>
@@ -199,7 +199,7 @@
     <t xml:space="preserve">SEC-CAT-INJ-001</t>
   </si>
   <si>
-    <t xml:space="preserve">The application must implement data entry validation measures before storing them to guarantee the integrity and security of the information.</t>
+    <t xml:space="preserve">La aplicación debe implementar medidas de validación de la entrada de datos antes de almacenarlos para garantizar la integridad y seguridad de la información procesada, almacenada o accesible a través de dispositivos de punto de usuario final. </t>
   </si>
   <si>
     <t xml:space="preserve">OWASP A03:2021, CWE-20, ISO/IEC 27002:2022 8.28</t>
@@ -211,7 +211,7 @@
     <t xml:space="preserve">SEC-CAT-INJ-002</t>
   </si>
   <si>
-    <t xml:space="preserve">The application must be secure against SQL injection attacks.</t>
+    <t xml:space="preserve">La aplicación debe ser segura frente a ataques de inyección SQL. Es necesario evitar posibles problemas de seguridad relacionados con la inyección SQL y ajustar la aplicación para eliminar cualquier riesgo asociado a este ataque. </t>
   </si>
   <si>
     <t xml:space="preserve">OWASP A03:2021, CWE-89, NIST SP 800-53 SI-10</t>
@@ -223,7 +223,7 @@
     <t xml:space="preserve">SEC-CAT-INJ-003</t>
   </si>
   <si>
-    <t xml:space="preserve">The application must implement effective restrictions on the types of files that users can upload.</t>
+    <t xml:space="preserve">La aplicación debe implementar restricciones efectivas sobre los tipos de archivos que los usuarios pueden cargar para evitar la carga de archivos peligrosos que puedan ser procesados automáticamente en el entorno de la aplicación. </t>
   </si>
   <si>
     <t xml:space="preserve">OWASP A08:2021, CWE-434, ISO/IEC 27002:2022 8.30</t>
@@ -235,7 +235,7 @@
     <t xml:space="preserve">SEC-CAT-INJ-004</t>
   </si>
   <si>
-    <t xml:space="preserve">The application must implement protection measures against command injections.</t>
+    <t xml:space="preserve">La aplicación debe implementar medidas de protección contra inyecciones de comandos. Dependiendo de la arquitectura de la aplicación, ésta debe ser modificada para escapar/sanitizar la entrada de caracteres especiales o configurar el sistema para proteger contra ataques de inyección de comandos. </t>
   </si>
   <si>
     <t xml:space="preserve">OWASP A03:2021, CWE-77, NIST SP 800-53 SI-10</t>
@@ -247,7 +247,7 @@
     <t xml:space="preserve">SEC-CAT-INJ-005</t>
   </si>
   <si>
-    <t xml:space="preserve">The application must implement protection measures against Cross-Site Scripting (XSS) vulnerabilities.</t>
+    <t xml:space="preserve">La aplicación debe implementar medidas de protección contra vulnerabilidades de Cross-Site Scripting (XSS) para prevenir ataques de inyección de código malicioso. </t>
   </si>
   <si>
     <t xml:space="preserve">OWASP A03:2021, CWE-79, ISO/IEC 27002:2022 8.28</t>
@@ -259,7 +259,7 @@
     <t xml:space="preserve">SEC-CAT-INJ-006</t>
   </si>
   <si>
-    <t xml:space="preserve">The application must implement an information output validation mechanism for reporting and data tables listing.</t>
+    <t xml:space="preserve">La aplicación debe implementar un mecanismo de validación de salida de información para los siguientes programas de software y/o aplicaciones: [informes listado de tablas de datos]. </t>
   </si>
   <si>
     <t xml:space="preserve">ISO/IEC 27002:2022 8.28, SIREN: validación de salida</t>
@@ -271,7 +271,7 @@
     <t xml:space="preserve">SEC-CAT-IND-001</t>
   </si>
   <si>
-    <t xml:space="preserve">The system must ensure that data is only processed following the directives provided in the data flow control.</t>
+    <t xml:space="preserve">El sistema debe garantizar que los datos sólo se procesan siguiendo las directivas proporcionadas en el control de flujo de datos. </t>
   </si>
   <si>
     <t xml:space="preserve">ISO/IEC 27002:2022 5.1, ISO 27799:2016, HIPAA §164.308(a)(3)</t>
@@ -283,7 +283,7 @@
     <t xml:space="preserve">SEC-CAT-IND-002</t>
   </si>
   <si>
-    <t xml:space="preserve">The system must implement measures to prevent unauthorized and involuntary transfer of information through shared system resources.</t>
+    <t xml:space="preserve">El sistema debe aplicar medidas para impedir la transferencia no autorizada e involuntaria de información a través de los recursos compartidos del sistema. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-53 SC-4, ISO/IEC 27002:2022 8.11</t>
@@ -295,7 +295,7 @@
     <t xml:space="preserve">SEC-CAT-IND-003</t>
   </si>
   <si>
-    <t xml:space="preserve">The application must show a system of use of the system and privacy notification before granting access.</t>
+    <t xml:space="preserve">La aplicación debe mostrar una notificación de uso del sistema y de privacidad antes de conceder el acceso. Este aviso debe contener información sobre la propiedad del sistema, la supervisión, registro y auditoría del uso, las sanciones por uso no autorizado y la aceptación de estas condiciones por parte del usuario. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-53 PL-4, AC-8, ISO/IEC 27002:2022 5.29</t>
@@ -307,7 +307,7 @@
     <t xml:space="preserve">SEC-CAT-IND-004</t>
   </si>
   <si>
-    <t xml:space="preserve">The system must generate error messages that provide the user with the information necessary for corrective actions without revealing exploitable details.</t>
+    <t xml:space="preserve">El sistema debe generar mensajes de error que proporcionen al usuario la información necesaria para realizar acciones correctivas sin revelar detalles que puedan ser explotados. </t>
   </si>
   <si>
     <t xml:space="preserve">OWASP A01:2021, CWE-209, NIST SP 800-53 SI-11</t>
@@ -319,7 +319,7 @@
     <t xml:space="preserve">SEC-CAT-IND-005</t>
   </si>
   <si>
-    <t xml:space="preserve">The application must physically or logically separate the functionality of the user from system management.</t>
+    <t xml:space="preserve">La aplicación debe separar física o lógicamente la funcionalidad del usuario, incluidos los servicios de interfaz de usuario y la funcionalidad de gestión del sistema. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-53 SC-2, AC-6, ISO/IEC 27002:2022 8.1</t>
@@ -331,7 +331,7 @@
     <t xml:space="preserve">SEC-CAT-IND-006</t>
   </si>
   <si>
-    <t xml:space="preserve">The application should be designed not to use emerging or non-categorized mobile code.</t>
+    <t xml:space="preserve">La aplicación debe estar diseñada para no utilizar código móvil emergente o no categorizado. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-53 SC-18, ISO/IEC 27002:2022 8.24</t>
@@ -343,7 +343,7 @@
     <t xml:space="preserve">SEC-CAT-IND-007</t>
   </si>
   <si>
-    <t xml:space="preserve">The application should not contain authentication data in its code or configuration files.</t>
+    <t xml:space="preserve">La aplicación no debe contener datos de autenticación incorporados en su código, archivos de configuración, scripts, archivos HTML o cualquier archivo ASCII. </t>
   </si>
   <si>
     <t xml:space="preserve">OWASP A07:2021, CWE-798, ISO/IEC 27002:2022 8.5</t>
@@ -355,7 +355,7 @@
     <t xml:space="preserve">SEC-CAT-IND-008</t>
   </si>
   <si>
-    <t xml:space="preserve">The application should not write sensitive data in the application records.</t>
+    <t xml:space="preserve">La aplicación no debe escribir datos sensibles en los registros de la aplicación. La aplicación debe diseñarse o reconfigurarse para evitar incluir datos sensibles en los registros. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-53 AU-9, ISO/IEC 27002:2022 8.31</t>
@@ -367,7 +367,7 @@
     <t xml:space="preserve">SEC-CAT-IND-009</t>
   </si>
   <si>
-    <t xml:space="preserve">The application should not unnecessarily store sensitive information in hidden fields.</t>
+    <t xml:space="preserve">La aplicación no debe almacenar o retener innecesariamente información sensible en campos ocultos. Es imprescindible eliminar esta información lo antes posible, o en su lugar, utilizar prácticas como el token o el truncado, siguiendo las directrices de PCI DSS para garantizar un almacenamiento seguro. </t>
   </si>
   <si>
     <t xml:space="preserve">PCI DSS Req. 3, OWASP A01:2021, ISO/IEC 27002:2022 8.7</t>
@@ -379,7 +379,7 @@
     <t xml:space="preserve">SEC-CAT-IND-010</t>
   </si>
   <si>
-    <t xml:space="preserve">The application must ensure that config/control files are not stored in the same directory as user data.</t>
+    <t xml:space="preserve">La aplicación debe garantizar que los archivos de configuración y control no se almacenan en el mismo directorio que los datos de usuario. Los datos de usuario de la aplicación deben estar ubicados en un directorio distinto del código de la aplicación, y deben establecerse permisos para los archivos de usuario a fin de restringir el acceso de los usuarios a la configuración de la aplicación. </t>
   </si>
   <si>
     <t xml:space="preserve">OWASP A05:2021, NIST SP 800-53 CM-5(3), ISO/IEC 27002:2022 8.9</t>
@@ -391,7 +391,7 @@
     <t xml:space="preserve">SEC-CAT-IND-011</t>
   </si>
   <si>
-    <t xml:space="preserve">The application should not be housed on a general-purpose server if designated critical.</t>
+    <t xml:space="preserve">La aplicación no debe alojarse en un servidor de propósito general si la aplicación es designada como crítica o de alta disponibilidad por el Oficial de Seguridad de la Información (ISSO). Las aplicaciones críticas no compartidas por otras aplicaciones menos críticas deben implementarse en servidores. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-53 SC-39, ISO/IEC 27002:2022 5.34</t>
@@ -403,7 +403,7 @@
     <t xml:space="preserve">SEC-CAT-IND-012</t>
   </si>
   <si>
-    <t xml:space="preserve">The application must implement an adequate limitation of access routes to prevent malicious route manipulation that can lead to unauthorized revelation of files or directories.</t>
+    <t xml:space="preserve">La aplicación debe implementar una limitación adecuada de las rutas de acceso para evitar la manipulación maliciosa de rutas que pueda conducir a la revelación no autorizada de archivos o directorios. </t>
   </si>
   <si>
     <t xml:space="preserve">OWASP A01:2021, CWE-22, ISO/IEC 27002:2022 8.9</t>
@@ -415,7 +415,7 @@
     <t xml:space="preserve">SEC-CAT-IND-013</t>
   </si>
   <si>
-    <t xml:space="preserve">The application must be protected against vulnerabilities of canonical representation.</t>
+    <t xml:space="preserve">La aplicación debe estar protegida contra vulnerabilidades de representación canónica. Se debe seleccionar una forma canónica adecuada y canonizar toda la entrada del usuario antes de tomar decisiones de autorización. </t>
   </si>
   <si>
     <t xml:space="preserve">CWE-180, CWE-179, NIST SP 800-53 SI-10</t>
@@ -427,7 +427,7 @@
     <t xml:space="preserve">SEC-CAT-IND-014</t>
   </si>
   <si>
-    <t xml:space="preserve">The application must incorporate a 'safe failure' approach through safe error management.</t>
+    <t xml:space="preserve">La aplicación debe incorporar un enfoque de "fallo seguro" mediante una gestión segura de errores para evitar vulnerabilidades derivadas de una gestión incorrecta de códigos de retorno y excepciones en todos los componentes del sistema. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-53 SI-11, ISO/IEC 27002:2022 8.32</t>
@@ -439,7 +439,7 @@
     <t xml:space="preserve">SEC-CAT-IND-015</t>
   </si>
   <si>
-    <t xml:space="preserve">The application should not be vulnerable to race conditions.</t>
+    <t xml:space="preserve">La aplicación no debe ser vulnerable a condiciones de carrera. </t>
   </si>
   <si>
     <t xml:space="preserve">CWE-362, NIST SP 800-53 SI-10</t>
@@ -451,7 +451,7 @@
     <t xml:space="preserve">SEC-CAT-IND-016</t>
   </si>
   <si>
-    <t xml:space="preserve">The application must implement measures to prevent memory use after being released.</t>
+    <t xml:space="preserve">La aplicación debe implementar medidas para prevenir el uso de memoria después de ser liberada ya que la referencia a memoria después de ser liberada puede causar fallos en el programa, el uso de valores inesperados, o ejecutar código no deseado. </t>
   </si>
   <si>
     <t xml:space="preserve">CWE-416, ISO/IEC 27002:2022 8.8</t>
@@ -463,7 +463,7 @@
     <t xml:space="preserve">SEC-CAT-IND-017</t>
   </si>
   <si>
-    <t xml:space="preserve">The application should prevent null pointer reference.</t>
+    <t xml:space="preserve">La aplicación debe prevenir la referencia a punteros nulos, evitando intentar acceder a un puntero nulo, lo que podría provocar fallos o salidas inesperadas. </t>
   </si>
   <si>
     <t xml:space="preserve">CWE-476, ISO/IEC 27002:2022 8.8</t>
@@ -475,7 +475,7 @@
     <t xml:space="preserve">SEC-CAT-IND-018</t>
   </si>
   <si>
-    <t xml:space="preserve">The application must implement controls defined by the organization to protect the system's memory against unauthorized code execution.</t>
+    <t xml:space="preserve">La aplicación debe implementar controles definidos por la organización para proteger la memoria del sistema contra la ejecución de código no autorizado. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-53 SI-16, ISO/IEC 27002:2022 8.8</t>
@@ -487,7 +487,7 @@
     <t xml:space="preserve">SEC-CAT-IND-019</t>
   </si>
   <si>
-    <t xml:space="preserve">The application should not be vulnerable to buffer overflow attacks.</t>
+    <t xml:space="preserve">La aplicación no debe ser vulnerable a ataques de desbordamiento de búfer. </t>
   </si>
   <si>
     <t xml:space="preserve">CWE-119, NIST SP 800-53 SI-10, ISO/IEC 27002:2022 8.8</t>
@@ -499,7 +499,7 @@
     <t xml:space="preserve">SEC-CAT-IND-020</t>
   </si>
   <si>
-    <t xml:space="preserve">The application should be designed to use components that are not vulnerable to XML attacks.</t>
+    <t xml:space="preserve">La aplicación debe diseñarse para utilizar componentes que no sean vulnerables a ataques XML. </t>
   </si>
   <si>
     <t xml:space="preserve">OWASP XML External Entity (XXE), CWE-611, ISO/IEC 27002:2022 8.30</t>
@@ -511,7 +511,7 @@
     <t xml:space="preserve">SEC-CAT-IND-021</t>
   </si>
   <si>
-    <t xml:space="preserve">The application must implement repetition-resistant authentication mechanisms for network access for privileged and non-privileged accounts.</t>
+    <t xml:space="preserve">La aplicación debe implementar mecanismos de autenticación resistentes a la repetición para el acceso a la red de cuentas con y sin privilegios. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-53 IA-2(8), ISO/IEC 27002:2022 8.2</t>
@@ -523,7 +523,7 @@
     <t xml:space="preserve">SEC-CAT-IND-022</t>
   </si>
   <si>
-    <t xml:space="preserve">Applications with SOAP messages requiring integrity must include: Message ID, Service Request, Timestamp, SAML Assertion (optional), all digitally signed.</t>
+    <t xml:space="preserve">Las aplicaciones con mensajes SOAP que requieran integridad deben incluir los siguientes elementos de mensaje: -ID del mensaje -Solicitud de servicio -Sello de fecha y hora -Aserción SAML (incluida opcionalmente en los mensajes), y todos los elementos del mensaje deben estar firmados digitalmente. </t>
   </si>
   <si>
     <t xml:space="preserve">WS-Security, NIST SP 800-95, ISO/IEC 27002:2022 10.4</t>
@@ -535,7 +535,7 @@
     <t xml:space="preserve">SEC-CAT-IND-023</t>
   </si>
   <si>
-    <t xml:space="preserve">The application must authenticate all endpoint devices before establishing any connection.</t>
+    <t xml:space="preserve">La aplicación debe autenticar todos los dispositivos terminales conectados a la red antes de establecer cualquier conexión. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-53 AC-17(1), ISO/IEC 27002:2022 5.15</t>
@@ -547,7 +547,7 @@
     <t xml:space="preserve">SEC-CAT-IND-024</t>
   </si>
   <si>
-    <t xml:space="preserve">Safe messages with WS-Security must have creation/expiration timestamps and sequence numbers.</t>
+    <t xml:space="preserve">Los mensajes seguros con WS-Security deben tener marcas de tiempo que indiquen cuando fueron creados y cuando expiraron. La aplicación debe estar diseñada para utilizar estas marcas de tiempo y números de secuencia en los mensajes WS-Security. </t>
   </si>
   <si>
     <t xml:space="preserve">WS-Security y NIST SP 800-95: Tiempos de vida y secuencia en mensajes seguros. ISO/IEC 27002:2022 10.4: Prevención de repeticiones y expiración de mensajes.</t>
@@ -556,7 +556,7 @@
     <t xml:space="preserve">SEC-CAT-IND-025</t>
   </si>
   <si>
-    <t xml:space="preserve">The application must verify validity periods in WS-Security or SAML messages.</t>
+    <t xml:space="preserve">La aplicación debe verificar los periodos de validez en todos los mensajes que utilicen declaraciones WS-SECURITY o SAML. Diseñe y configure la aplicación para utilizar y verificar los periodos de validez en todos los perfiles de token WS-Security y declaraciones SAML. </t>
   </si>
   <si>
     <t xml:space="preserve">SAML 2.0 Core, WS-Security, ISO/IEC 27002:2022 10.4</t>
@@ -568,7 +568,7 @@
     <t xml:space="preserve">SEC-CAT-SEM-001</t>
   </si>
   <si>
-    <t xml:space="preserve">The application must define, document, and implement configurations adjusted restrictively with operational needs.</t>
+    <t xml:space="preserve">La aplicación debe definir, documentar e implementar configuraciones, incluyendo seguridad, hardware, software, servicios y redes, ajustándolas de la forma más restrictiva consistente con los requerimientos operacionales. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-53 CM-2, ISO/IEC 27002:2022 5.14</t>
@@ -580,7 +580,7 @@
     <t xml:space="preserve">SEC-CAT-SEM-002</t>
   </si>
   <si>
-    <t xml:space="preserve">The application must define and implement due security settings to avoid DDoS attacks.</t>
+    <t xml:space="preserve">La aplicación debe definir e implementar las debidas configuraciones de seguridad para evitar ataques DDoS. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-53 SC-5, ISO/IEC 27002:2022 8.16</t>
@@ -592,7 +592,7 @@
     <t xml:space="preserve">SEC-CAT-SEM-003</t>
   </si>
   <si>
-    <t xml:space="preserve">The application must validate deserialization of non-reliable data before processing.</t>
+    <t xml:space="preserve">La aplicación debe implementar medidas para validar la deserialización de datos no fiables y garantizar que los datos resultantes son válidos antes de procesarlos. </t>
   </si>
   <si>
     <t xml:space="preserve">OWASP A08:2021, CWE-502, ISO/IEC 27002:2022 8.28</t>
@@ -604,7 +604,7 @@
     <t xml:space="preserve">SEC-CAT-SEM-004</t>
   </si>
   <si>
-    <t xml:space="preserve">The application must be protected against CSRF through tokens, referrer validation and additional controls.</t>
+    <t xml:space="preserve">La aplicación debe estar protegida contra las vulnerabilidades de FORJACIÓN DE SOLICITUDES CROSS-SITE (CSRF) mediante la configuración para utilizar tokens de desafío impredecibles y verificar la referencia HTTP garantizando que la solicitud se emitió desde el propio sitio. Además deben implementarse los controles de mitigación necesarios como el uso de servicios de reputación web </t>
   </si>
   <si>
     <t xml:space="preserve">OWASP A05:2021, CWE-352, ISO/IEC 27002:2022 8.28</t>
@@ -616,7 +616,7 @@
     <t xml:space="preserve">SEC-CAT-SEM-005</t>
   </si>
   <si>
-    <t xml:space="preserve">The application must be configured to deactivate non-essential capabilities.</t>
+    <t xml:space="preserve">La aplicación debe configurarse para desactivar las capacidades no esenciales. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-53 CM-7, ISO/IEC 27002:2022 8.9</t>
@@ -628,7 +628,7 @@
     <t xml:space="preserve">SEC-CAT-SEM-006</t>
   </si>
   <si>
-    <t xml:space="preserve">The application should avoid showing users what is not required, including architecture in error events.</t>
+    <t xml:space="preserve">La aplicación debe evitar mostrar a los usuarios lo que no sea necesario. Es necesario configurarla para que no revele detalles técnicos sobre la arquitectura en eventos de error. </t>
   </si>
   <si>
     <t xml:space="preserve">OWASP A01:2021, CWE-209, ISO/IEC 27002:2022 8.32</t>
@@ -640,7 +640,7 @@
     <t xml:space="preserve">SEC-CAT-SEM-007</t>
   </si>
   <si>
-    <t xml:space="preserve">The application must identify and authenticate uniquely non-organizational users (or processes that act in their name).</t>
+    <t xml:space="preserve">La aplicación debe identificar y autenticar de forma única a los usuarios no organizativos (o procesos que actúen en nombre de usuarios no organizativos). </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-53 IA-8, ISO/IEC 27002:2022 5.16</t>
@@ -652,7 +652,7 @@
     <t xml:space="preserve">SEC-CAT-SEM-008</t>
   </si>
   <si>
-    <t xml:space="preserve">The application must identify and authenticate uniquely organizational users (or processes that act in their name).</t>
+    <t xml:space="preserve">La aplicación debe identificar y autenticar de forma única a los usuarios de la organización (o procesos que actúen en nombre de usuarios de la organización). </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-53 IA-2, ISO/IEC 27002:2022 5.16</t>
@@ -664,7 +664,7 @@
     <t xml:space="preserve">SEC-CAT-SEM-009</t>
   </si>
   <si>
-    <t xml:space="preserve">Applications issuing SAML statements must use FIPS-approved random numbers for SAML session generation.</t>
+    <t xml:space="preserve">Las aplicaciones que emiten declaraciones SAML deben utilizar números aleatorios aprobados por FIPS para generar sesiones SAML en el elemento AuthnStatement de Saml </t>
   </si>
   <si>
     <t xml:space="preserve">FIPS 140-2, NIST SP 800-133, SAML 2.0 Core</t>
@@ -676,7 +676,7 @@
     <t xml:space="preserve">SEC-CAT-SEM-010</t>
   </si>
   <si>
-    <t xml:space="preserve">Each asserting party must provide unique identifiers for each SAML statement.</t>
+    <t xml:space="preserve">La aplicación debe garantizar que cada parte que emite declaraciones (Asserting Party) proporciona identificadores únicos para cada declaración SAML (Security Assertion Markup Language). Se requiere diseñar y configurar cada autoridad de afirmación SAML para utilizar identificadores de afirmación únicos. </t>
   </si>
   <si>
     <t xml:space="preserve">SAML 2.0 Core, NIST SP 800-95</t>
@@ -688,7 +688,7 @@
     <t xml:space="preserve">SEC-CAT-SEM-011</t>
   </si>
   <si>
-    <t xml:space="preserve">Guarantee encrypted statements or equivalent confidentiality protections during intermediary transmission.</t>
+    <t xml:space="preserve">La aplicación debe garantizar el uso de declaraciones cifradas o protecciones de confidencialidad equivalentes cuando los datos de la declaración se transmiten a través de un intermediario, y la confidencialidad de las declaraciones de declaraciones es necesaria durante la transmisión a través del intermediario. </t>
   </si>
   <si>
     <t xml:space="preserve">SAML 2.0 Bindings, WS-Security, ISO/IEC 27002:2022 10.1</t>
@@ -700,7 +700,7 @@
     <t xml:space="preserve">SEC-CAT-SEM-012</t>
   </si>
   <si>
-    <t xml:space="preserve">Use &lt;NotBefore&gt;, &lt;NotOnOrAfter&gt;, and &lt;OneTimeUse&gt; with &lt;Conditions&gt; in SAML Assertions.</t>
+    <t xml:space="preserve">La aplicación debe utilizar tanto los elementos &lt;NotBefore&gt; y &lt;NotOnOrAfter&gt; como el elemento &lt;OneTimeUse&gt; cuando utilice el elemento &lt;Conditions&gt; en una aserción SAML. </t>
   </si>
   <si>
     <t xml:space="preserve">SAML 2.0 Core §2.5.1</t>
@@ -712,7 +712,7 @@
     <t xml:space="preserve">SEC-CAT-SEM-013</t>
   </si>
   <si>
-    <t xml:space="preserve">Use NotOnOrAfter condition with SubjectConfirmation in SAML assertion.</t>
+    <t xml:space="preserve">La aplicación debe utilizar la condición NotOnOrAfter cuando utilice el elemento SubjectConfirmation en una aserción SAML. </t>
   </si>
   <si>
     <t xml:space="preserve">SAML 2.0 Core §2.4.1.4</t>
@@ -724,7 +724,7 @@
     <t xml:space="preserve">SEC-CAT-SEM-014</t>
   </si>
   <si>
-    <t xml:space="preserve">Configure session cookies with HTTPOnly and Secure flags.</t>
+    <t xml:space="preserve">La aplicación debe configurar las cookies de sesión con las siguientes propiedades: o Establecer la bandera HTTPOnly en las cookies de sesión. o Asegurarse de que la bandera segura (Secure) está activada en las cookies de sesión. </t>
   </si>
   <si>
     <t xml:space="preserve">OWASP A07:2021, ISO/IEC 27002:2022 8.31</t>
@@ -736,7 +736,7 @@
     <t xml:space="preserve">SEC-CAT-VOC-001</t>
   </si>
   <si>
-    <t xml:space="preserve">Keep updated on the components or libraries of the application.</t>
+    <t xml:space="preserve">Mantener actualizados los componentes o librerías de la aplicación. </t>
   </si>
   <si>
     <t xml:space="preserve">OWASP A06:2021, ISO/IEC 27002:2022 8.34</t>
@@ -748,7 +748,7 @@
     <t xml:space="preserve">SEC-CAT-VOC-002</t>
   </si>
   <si>
-    <t xml:space="preserve">Remove or replace unsupported libraries or components.</t>
+    <t xml:space="preserve">Las librerías o componentes de software que no cuenten con el soporte o mantenimiento deben ser eliminados o sustituidos. </t>
   </si>
   <si>
     <t xml:space="preserve">OWASP A06:2021: Riesgo de bibliotecas obsoletas. ISO/IEC 27002:2022 8.34: Eliminación de componentes sin soporte o desactualizados.</t>
@@ -757,7 +757,7 @@
     <t xml:space="preserve">SEC-CAT-VOC-003</t>
   </si>
   <si>
-    <t xml:space="preserve">The application must provide notifications or alerts when product updates and safety-related patches are available.</t>
+    <t xml:space="preserve">La aplicación debe proporcionar notificaciones o alertas cuando estén disponibles actualizaciones del producto y parches relacionados con la seguridad. </t>
   </si>
   <si>
     <t xml:space="preserve">ISO/IEC 27002:2022 8.33, NIST SP 800-40</t>
@@ -769,7 +769,7 @@
     <t xml:space="preserve">SEC-CAT-IAF-001</t>
   </si>
   <si>
-    <t xml:space="preserve">The application must identify user actions that can be carried out without requiring identification or authentication.</t>
+    <t xml:space="preserve">La aplicación debe identificar las acciones de usuario que pueden llevarse a cabo en el sistema sin necesidad de identificación o autenticación. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-53 AC-14, ISO/IEC 27002:2022 5.16</t>
@@ -781,7 +781,7 @@
     <t xml:space="preserve">SEC-CAT-IAF-002</t>
   </si>
   <si>
-    <t xml:space="preserve">Organizations must submit EHRI-linked POS users to a formal registration process.</t>
+    <t xml:space="preserve">Todas las organizaciones que se conecten al Sistema de Información del Registro Electrónico Sanitario (EHRI) deben someter a los posibles usuarios de Sistemas Punto de Venta (POS) que se conecten a EHRI a un proceso formal de registro de Usuarios. </t>
   </si>
   <si>
     <t xml:space="preserve">ISO/IEC 27002:2022 5.18, HIPAA §164.308(a)(3)(ii)(A)</t>
@@ -793,7 +793,7 @@
     <t xml:space="preserve">SEC-CAT-IAF-003</t>
   </si>
   <si>
-    <t xml:space="preserve">PKI-based authentication must validate certificates by building a certification chain to an accepted trust anchor.</t>
+    <t xml:space="preserve">La aplicación, cuando utilice autenticación basada en PKI, debe validar los certificados construyendo una cadena de certificación (incluyendo información de estado) hacia un anclaje de confianza aceptado, por lo que la aplicación debe estar diseñada para crear una cadena de certificación hacia un Anclaje de Confianza aceptado cuando utilice autenticación basada en PKI. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-57, FIPS 140-2, ISO/IEC 27002:2022 10.1</t>
@@ -805,7 +805,7 @@
     <t xml:space="preserve">SEC-CAT-IAF-004</t>
   </si>
   <si>
-    <t xml:space="preserve">PKI-based authentication must enforce authorized access to private keys.</t>
+    <t xml:space="preserve">La aplicación, cuando utilice autenticación basada en infraestructura de clave pública (PKI), debe garantizar el acceso autorizado a la clave privada correspondiente, por lo que la aplicación o el mecanismo de control de acceso pertinente debe estar configurado para garantizar el acceso autorizado a la(s) clave(s) privada(s) de la aplicación. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-57, ISO/IEC 27002:2022 10.10</t>
@@ -817,7 +817,7 @@
     <t xml:space="preserve">SEC-CAT-IAF-005</t>
   </si>
   <si>
-    <t xml:space="preserve">The application must verify that the person/entity requesting access to ePHI is who they claim to be.</t>
+    <t xml:space="preserve">La aplicación debe implantar procedimientos para verificar que la persona o entidad que pretende acceder a la información sanitaria electrónica protegida es quien dice ser. </t>
   </si>
   <si>
     <t xml:space="preserve">HIPAA §164.312(d), ISO/IEC 27002:2022 5.17</t>
@@ -829,7 +829,7 @@
     <t xml:space="preserve">SEC-CAT-IAF-006</t>
   </si>
   <si>
-    <t xml:space="preserve">Impose 3 invalid login attempts in 15 min, block account for 1 hour, or until admin release.</t>
+    <t xml:space="preserve">La aplicación debe imponer un límite de 3 intentos de inicio de sesión no válidos por parte de un usuario durante 15 minutos y bloquear automáticamente la cuenta durante 1 hora; bloquear la cuenta o el nodo hasta que un administrador lo libere; retrasar el siguiente aviso de inicio de sesión durante 1 hora; notificar al administrador del sistema; adoptar el bloqueo permanente de la cuenta cuando se supere el número máximo de intentos fallidos. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-53 AC-7, ISO/IEC 27002:2022 5.17</t>
@@ -847,7 +847,7 @@
     <t xml:space="preserve">SEC-CAT-IAF-008</t>
   </si>
   <si>
-    <t xml:space="preserve">Implement multifactor authentication with at least two factors (e.g., CAC, token).</t>
+    <t xml:space="preserve">La aplicación debe implementar una autenticación multifactor robusta, utilizando al menos dos factores de autenticación (por ejemplo, CAC, Alt. Token) para acceder a redes y cuentas no privilegiadas. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-53 IA-2(1), ISO/IEC 27002:2022 5.17</t>
@@ -859,7 +859,7 @@
     <t xml:space="preserve">SEC-CAT-IAF-009</t>
   </si>
   <si>
-    <t xml:space="preserve">Allow single identity credential (single login) for patients or providers accessing other services.</t>
+    <t xml:space="preserve">La aplicación debe permitir a los usuarios utilizar una única credencial de identidad (login único), ya sean pacientes o proveedores, cuando el portal proporcione acceso a otras aplicaciones o servicios con mecanismos de autenticación independientes. </t>
   </si>
   <si>
     <t xml:space="preserve">ISO/IEC 27002:2022 5.17, NIST SP 800-63</t>
@@ -871,7 +871,7 @@
     <t xml:space="preserve">SEC-CAT-IAF-010</t>
   </si>
   <si>
-    <t xml:space="preserve">The application must select robust levels of identity assurance based on user roles.</t>
+    <t xml:space="preserve">La aplicación debe considerar y seleccionar niveles robustos de garantía de identidad siguiendo los roles de los usuarios, definiendo los mecanismos necesarios para probar la identidad del registro inicialmente. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-63-3, ISO/IEC 27002:2022 5.17</t>
@@ -889,7 +889,7 @@
     <t xml:space="preserve">SEC-CAT-IAF-012</t>
   </si>
   <si>
-    <t xml:space="preserve">The application must implement login procedures that protect against brute force attempts.</t>
+    <t xml:space="preserve">La aplicación debe implementar procedimientos de login seguros que protejan contra intentos de login por fuerza bruta. </t>
   </si>
   <si>
     <t xml:space="preserve">OWASP A07:2021, NIST SP 800-53 AC-7, ISO/IEC 27002:2022 5.17</t>
@@ -901,7 +901,7 @@
     <t xml:space="preserve">SEC-CAT-IAF-013</t>
   </si>
   <si>
-    <t xml:space="preserve">The application should ensure at least two authentication factors are used.</t>
+    <t xml:space="preserve">La aplicación debe considerar que al autenticar al usuario se implementan al menos los dos factores del mecanismo de autenticación. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST IA-2(1): Autenticación multifactor. ISO/IEC 27002:2022 5.17: Incorporación de múltiples factores de autenticación.</t>
@@ -910,7 +910,7 @@
     <t xml:space="preserve">SEC-CAT-IAF-014</t>
   </si>
   <si>
-    <t xml:space="preserve">Require re-authentication when authenticators, roles, or system security change.</t>
+    <t xml:space="preserve">La aplicación debe requerir la reautenticación de usuarios y dispositivos cuando cambien los autenticadores, roles o categorías de seguridad de los sistemas de información. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-53 IA-11, ISO/IEC 27002:2022 5.17</t>
@@ -922,7 +922,7 @@
     <t xml:space="preserve">SEC-CAT-IAF-015</t>
   </si>
   <si>
-    <t xml:space="preserve">Error messages during login should not offer specific help to unauthorized users.</t>
+    <t xml:space="preserve">En caso de error durante el inicio de sesión, la aplicación no debe ofrecer mensajes de ayuda específicos que puedan beneficiar a un usuario no autorizado. </t>
   </si>
   <si>
     <t xml:space="preserve">CWE-209, ISO/IEC 27002:2022 8.32</t>
@@ -934,7 +934,7 @@
     <t xml:space="preserve">SEC-CAT-IAF-016</t>
   </si>
   <si>
-    <t xml:space="preserve">Do not show system/application identifiers until login is complete.</t>
+    <t xml:space="preserve">La aplicación no debería mostrar identificadores del sistema o de la aplicación hasta que el proceso de inicio de sesión se haya completado con éxito. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-53 AC-8, ISO/IEC 27002:2022 8.9</t>
@@ -946,7 +946,7 @@
     <t xml:space="preserve">SEC-CAT-IAF-017</t>
   </si>
   <si>
-    <t xml:space="preserve">Passwords should not be transmitted in clear text over a network.</t>
+    <t xml:space="preserve">La aplicación no debe permitir que las contraseñas se transmitan en texto claro en una red, siguiendo la sección 9.4.2 J) de procedimientos de inicio de sesión seguro. </t>
   </si>
   <si>
     <t xml:space="preserve">ISO/IEC 27002:2022 8.27, OWASP A02:2021</t>
@@ -958,7 +958,7 @@
     <t xml:space="preserve">SEC-CAT-IAF-018</t>
   </si>
   <si>
-    <t xml:space="preserve">Passwords should not be shown during input in login procedures.</t>
+    <t xml:space="preserve">Durante los procedimientos de inicio de sesión, la aplicación no debería mostrar la contraseña que se está introduciendo. </t>
   </si>
   <si>
     <t xml:space="preserve">ISO/IEC 27002:2022 8.27</t>
@@ -970,7 +970,7 @@
     <t xml:space="preserve">SEC-CAT-IAF-019</t>
   </si>
   <si>
-    <t xml:space="preserve">Prohibit password reuse for at least five generations.</t>
+    <t xml:space="preserve">La aplicación debe prohibir la reutilización de contraseñas durante un mínimo de cinco generaciones. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-63B §5.1.1.2, ISO/IEC 27002:2022 8.27</t>
@@ -982,7 +982,7 @@
     <t xml:space="preserve">SEC-CAT-IAF-020</t>
   </si>
   <si>
-    <t xml:space="preserve">Allow use of a temporary password that must be changed immediately.</t>
+    <t xml:space="preserve">La aplicación debe permitir el uso de una contraseña temporal para la sesión en el sistema, con un cambio inmediato a una contraseña permanente. </t>
   </si>
   <si>
     <t xml:space="preserve">ISO/IEC 27002:2022 8.2, NIST SP 800-63B §5.1.1.2</t>
@@ -994,7 +994,7 @@
     <t xml:space="preserve">SEC-CAT-IAF-021</t>
   </si>
   <si>
-    <t xml:space="preserve">After login, show last successful login and any attempts since.</t>
+    <t xml:space="preserve">La aplicación debe, cuando se complete un inicio de sesión con éxito, mostrar la siguiente información: 1. Fecha y hora del último inicio de sesión con éxito. 2. Detalles de cualquier inicio de sesión e intentos de inicio de sesión desde la última sesión correcta. </t>
   </si>
   <si>
     <t xml:space="preserve">ISO/IEC 27002:2022 5.18, NIST SP 800-53 AC-9</t>
@@ -1006,7 +1006,7 @@
     <t xml:space="preserve">SEC-CAT-IAF-022</t>
   </si>
   <si>
-    <t xml:space="preserve">Minimum 24-hour password life policy.</t>
+    <t xml:space="preserve">La aplicación debe aplicar una política de vida mínima de la contraseña de 24 horas/1 día. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-53 IA-5(1), ISO/IEC 27002:2022 8.2</t>
@@ -1021,7 +1021,7 @@
     <t xml:space="preserve">SEC-CAT-IAF-023</t>
   </si>
   <si>
-    <t xml:space="preserve">Maximum 60-day password lifetime.</t>
+    <t xml:space="preserve">La aplicación debe aplicar una restricción de contraseña máxima de 60 días. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-63B, ISO/IEC 27002:2022 8.2</t>
@@ -1033,7 +1033,7 @@
     <t xml:space="preserve">SEC-CAT-IAF-024</t>
   </si>
   <si>
-    <t xml:space="preserve">Password change must involve at least eight character changes.</t>
+    <t xml:space="preserve">La aplicación debe garantizar que el cambio de contraseña requiera el cambio de al menos ocho caracteres. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-63B §5.1.1.2 (parcial), ISO/IEC 27002:2022 8.2</t>
@@ -1045,7 +1045,7 @@
     <t xml:space="preserve">SEC-CAT-IAF-025</t>
   </si>
   <si>
-    <t xml:space="preserve">Password complexity: 15 characters, at least one upper, lower, numeric, and special character.</t>
+    <t xml:space="preserve">La aplicación debe cumplir las siguientes políticas de complejidad de contraseñas: o Exigir al menos un carácter especial. o Aplicar una longitud mínima de contraseña de 15 caracteres. o Exigir al menos un carácter en mayúscula. o Exigir al menos un carácter en minúscula. o Imponer la complejidad de la contraseña exigiendo al menos un carácter numérico. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST 800-63B §5.1.1.2: Longitud y complejidad en autenticadores secretos. ISO/IEC 27002:2022 8.2: Complejidad y robustez de contraseñas.</t>
@@ -1054,7 +1054,7 @@
     <t xml:space="preserve">SEC-CAT-IAF-026</t>
   </si>
   <si>
-    <t xml:space="preserve">Only user or administrator can change passwords.</t>
+    <t xml:space="preserve">La aplicación debe impedir que los usuarios, excepto el administrador o el usuario asociado a la contraseña, realicen cambios de contraseña. </t>
   </si>
   <si>
     <t xml:space="preserve">ISO/IEC 27002:2022 5.17</t>
@@ -1066,7 +1066,7 @@
     <t xml:space="preserve">SEC-CAT-IAF-027</t>
   </si>
   <si>
-    <t xml:space="preserve">Do not implement default or pre-set credentials, especially for administrators.</t>
+    <t xml:space="preserve">No envíe ni implemente credenciales predeterminadas especialmente para administradores </t>
   </si>
   <si>
     <t xml:space="preserve">OWASP A07:2021, ISO/IEC 27002:2022 8.2</t>
@@ -1078,7 +1078,7 @@
     <t xml:space="preserve">SEC-CAT-IAF-028</t>
   </si>
   <si>
-    <t xml:space="preserve">Limit concurrent sessions to three per account.</t>
+    <t xml:space="preserve">La aplicación debe limitar a tres el número de sesiones concurrentes para cada cuenta. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-53 AC-10, ISO/IEC 27002:2022 8.30</t>
@@ -1096,7 +1096,7 @@
     <t xml:space="preserve">SEC-CAT-IAF-030</t>
   </si>
   <si>
-    <t xml:space="preserve">Restrict duration of connections to application services to enhance access security.</t>
+    <t xml:space="preserve">La aplicación EHRI debe restringir la duración de las conexiones a los servicios de aplicación para proporcionar seguridad adicional en el acceso a dichas aplicaciones. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-53 AC-12, ISO/IEC 27002:2022 8.30</t>
@@ -1108,7 +1108,7 @@
     <t xml:space="preserve">SEC-CAT-IAF-031</t>
   </si>
   <si>
-    <t xml:space="preserve">Automatically terminate session after default inactivity period.</t>
+    <t xml:space="preserve">La aplicación debe implementar procedimientos electrónicos que finalicen automáticamente una sesión electrónica tras un periodo de inactividad predeterminado. </t>
   </si>
   <si>
     <t xml:space="preserve">HIPAA §164.312(b), NIST SP 800-53 AC-12, ISO/IEC 27002:2022 8.30</t>
@@ -1120,7 +1120,7 @@
     <t xml:space="preserve">SEC-CAT-IAF-032</t>
   </si>
   <si>
-    <t xml:space="preserve">End administrator session after 10 minutes of inactivity.</t>
+    <t xml:space="preserve">La aplicación debe finalizar automáticamente la sesión del usuario administrador y cerrar la sesión del administrador una vez transcurrido un periodo de inactividad de 10 minutos. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-53 AC-12(1), ISO/IEC 27002:2022 8.30</t>
@@ -1132,7 +1132,7 @@
     <t xml:space="preserve">SEC-CAT-IAF-033</t>
   </si>
   <si>
-    <t xml:space="preserve">End non-privileged user session after 15 minutes of inactivity.</t>
+    <t xml:space="preserve">La aplicación debe finalizar automáticamente la sesión de usuario sin privilegios y cerrar la sesión de los usuarios sin privilegios una vez transcurrido un periodo de inactividad de 15 minutos. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST AC-12: Cierre de sesión por inactividad. ISO/IEC 27002:2022 8.30: Control de sesiones inactivas.</t>
@@ -1141,13 +1141,16 @@
     <t xml:space="preserve">SEC-CAT-IAF-034</t>
   </si>
   <si>
+    <t xml:space="preserve">La aplicación debe finalizar automáticamente la sesión de usuario sin privilegios y cerrar la sesión de usuarios sin privilegios una vez transcurrido un periodo de inactividad de 15 minutos. </t>
+  </si>
+  <si>
     <t xml:space="preserve">NIST AC-12: Requiere finalización automática. ISO/IEC 27002:2022 8.30: Prevención de sesiones huérfanas.</t>
   </si>
   <si>
     <t xml:space="preserve">SEC-CAT-IAF-035</t>
   </si>
   <si>
-    <t xml:space="preserve">Ensure session cleanup: close network connections, destroy session ID and cookies.</t>
+    <t xml:space="preserve">La aplicación debe garantizar que, al final de una sesión, se cierren todas las conexiones de red vinculadas a esa sesión y se destruyan el identificador de sesión y los datos de las cookies. </t>
   </si>
   <si>
     <t xml:space="preserve">OWASP A07:2021, NIST SP 800-53 SC-23, ISO/IEC 27002:2022 8.30</t>
@@ -1159,7 +1162,7 @@
     <t xml:space="preserve">SEC-CAT-IAF-036</t>
   </si>
   <si>
-    <t xml:space="preserve">Revoke user access privileges immediately upon deauthorization.</t>
+    <t xml:space="preserve">La aplicación debe ser capaz de revocar a tiempo los privilegios de acceso del usuario, lo que implica impedir inmediatamente que el usuario acceda al sistema una vez revocados sus privilegios. </t>
   </si>
   <si>
     <t xml:space="preserve">HIPAA §164.308(a)(3)(ii)(C), NIST SP 800-53 AC-2(5), ISO/IEC 27002:2022 5.18</t>
@@ -1171,7 +1174,7 @@
     <t xml:space="preserve">SEC-CAT-IAF-037</t>
   </si>
   <si>
-    <t xml:space="preserve">Close user sessions when accounts are deleted.</t>
+    <t xml:space="preserve">La aplicación debe finalizar las sesiones de usuario existentes eliminando una cuenta. Configure la aplicación para cerrar las sesiones de usuario cuyas cuentas se hayan eliminado. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-53 AC-2(3), ISO/IEC 27002:2022 5.18</t>
@@ -1183,7 +1186,7 @@
     <t xml:space="preserve">SEC-CAT-IAF-038</t>
   </si>
   <si>
-    <t xml:space="preserve">Automatically delete/deactivate temporary accounts after 72 hours.</t>
+    <t xml:space="preserve">La aplicación debe eliminar o desactivar automáticamente las cuentas de usuario temporales 72 horas después de su creación. Configure las cuentas temporales para que se eliminen o desactiven automáticamente después de 72 horas de su creación. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-53 AC-2(2), ISO/IEC 27002:2022 5.18</t>
@@ -1195,7 +1198,7 @@
     <t xml:space="preserve">SEC-CAT-IAF-039</t>
   </si>
   <si>
-    <t xml:space="preserve">Deactivate user accounts after 35 days of inactivity.</t>
+    <t xml:space="preserve">La aplicación debe desactivar automáticamente las cuentas de usuario después de un período de inactividad de 35 días. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST AC-2(3): Inactividad prolongada activa desactivación. ISO/IEC 27002:2022 5.18: Periodos de uso deben ser controlados.</t>
@@ -1204,7 +1207,7 @@
     <t xml:space="preserve">SEC-CAT-SDF-001</t>
   </si>
   <si>
-    <t xml:space="preserve">Acquire components only from official sources using signed packages.</t>
+    <t xml:space="preserve">La aplicación debe adquirir componentes únicamente de fuentes oficiales a través de enlaces seguros. Se debe dar preferencia a los paquetes firmados para reducir la posibilidad de incluir un componente modificado o malicioso. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-218, ISO/IEC 27002:2022 8.25</t>
@@ -1216,7 +1219,7 @@
     <t xml:space="preserve">SEC-CAT-SDF-002</t>
   </si>
   <si>
-    <t xml:space="preserve">Use software supply chain safety tools to verify components for known vulnerabilities.</t>
+    <t xml:space="preserve">La aplicación debe incorporar una herramienta de seguridad de la cadena de suministro de software para verificar que los componentes no contengan vulnerabilidades conocidas. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-218: Uso de escaneo automatizado de componentes. ISO/IEC 27002:2022 8.25: Validación de integridad y seguridad de software externo.</t>
@@ -1225,7 +1228,7 @@
     <t xml:space="preserve">SEC-CAT-SDF-003</t>
   </si>
   <si>
-    <t xml:space="preserve">Review code and config changes to prevent malicious code in pipeline.</t>
+    <t xml:space="preserve">La aplicación debe contar con un proceso para revisar el código y los cambios de configuración a fin de minimizar la posibilidad de introducción de código malicioso o de configuración en el flujo de trabajo del software </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-218, ISO/IEC 27002:2022 8.29</t>
@@ -1237,7 +1240,7 @@
     <t xml:space="preserve">SEC-CAT-SDF-004</t>
   </si>
   <si>
-    <t xml:space="preserve">Ensure CI/CD channels have proper segregation and access controls.</t>
+    <t xml:space="preserve">La aplicación debe garantizar que su canal de integración continua/implementación continua (CI/CD) cuente con la segregación configuración segura y control de acceso adecuados para garantizar la integridad del código que fluye a través de los procesos de construcción e implementación </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-218: Separación de entornos y control de acceso en la canalización. ISO/IEC 27002:2022 8.29: Protección de entornos de desarrollo y entrega continua.</t>
@@ -1246,7 +1249,7 @@
     <t xml:space="preserve">SEC-CAT-SDF-005</t>
   </si>
   <si>
-    <t xml:space="preserve">Do not send non-signed or non-encrypted serialized data to unreliable clients without integrity checks.</t>
+    <t xml:space="preserve">La aplicación debe garantizar que los datos serializados no firmados ni cifrados no se envíen a clientes no confiables sin verificación de integridad o firma digital para detectar manipulaciones o reproducciones de los datos serializados </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-53 SC-12, ISO/IEC 27002:2022 10.1</t>
@@ -1258,7 +1261,7 @@
     <t xml:space="preserve">SEC-CAT-SDF-006</t>
   </si>
   <si>
-    <t xml:space="preserve">Show historical record content, including who accessed or modified and when.</t>
+    <t xml:space="preserve">La aplicación debe poder mostrar el contenido previo de un registro en cualquier momento así como los detalles asociados de quién ingresó aceptó o modificó los datos y en qué momento </t>
   </si>
   <si>
     <t xml:space="preserve">HIPAA §164.312(b), ISO/IEC 27002:2022 8.15</t>
@@ -1270,7 +1273,7 @@
     <t xml:space="preserve">SEC-CAT-SDF-007</t>
   </si>
   <si>
-    <t xml:space="preserve">Implement policies to protect EPHI against alteration or destruction.</t>
+    <t xml:space="preserve">La aplicación debe implementar políticas y procedimientos para proteger la información electrónica de salud protegida (EPHI) contra alteraciones o destrucciones indebidas </t>
   </si>
   <si>
     <t xml:space="preserve">HIPAA §164.312(c)(1), ISO/IEC 27002:2022 8.14</t>
@@ -1282,7 +1285,7 @@
     <t xml:space="preserve">SEC-CAT-LMF-001</t>
   </si>
   <si>
-    <t xml:space="preserve">Implement comprehensive security management to ensure ePHI confidentiality, integrity, and availability; include system activity review.</t>
+    <t xml:space="preserve">La aplicación debe implementar un proceso integral de gestión de seguridad para garantizar el no repudio la confidencialidad la integridad y la disponibilidad de toda la información electrónica de salud protegida (EPHI) creada recibida mantenida o transmitida. Este proceso debe incluir la revisión periódica de los registros de actividad del sistema como registros de auditoría informes de acceso e informes de monitoreo de seguridad </t>
   </si>
   <si>
     <t xml:space="preserve">HIPAA §164.308(a)(1)(ii)(D), ISO/IEC 27002:2022 5.10</t>
@@ -1294,16 +1297,13 @@
     <t xml:space="preserve">SEC-CAT-LMF-002</t>
   </si>
   <si>
-    <t xml:space="preserve">Implement comprehensive security management process for ePHI (repetido de LMF-001).</t>
-  </si>
-  <si>
     <t xml:space="preserve">HIPAA §164.308(a)(1)(ii)(D): Análisis de actividad como parte de gestión de riesgos. ISO/IEC 27002:2022 5.10: Supervisión y ajuste de controles de seguridad.</t>
   </si>
   <si>
     <t xml:space="preserve">SEC-CAT-LMF-003</t>
   </si>
   <si>
-    <t xml:space="preserve">Application must support audit reduction for incident investigations.</t>
+    <t xml:space="preserve">La aplicación debe tener una capacidad de reducción de auditorías que facilite la investigación tras incidentes de seguridad. La aplicación debe estar configurada para ofrecer una capacidad de reducción de auditorías que facilite las investigaciones forenses </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-92, ISO/IEC 27002:2022 5.10</t>
@@ -1315,7 +1315,7 @@
     <t xml:space="preserve">SEC-CAT-LMF-004</t>
   </si>
   <si>
-    <t xml:space="preserve">Audit successful/unsuccessful privilege grant attempts.</t>
+    <t xml:space="preserve">La aplicación debe generar registros de auditoría cuando se realizan intentos exitosos o fallidos de otorgar privilegios. Configure la aplicación para auditar los intentos exitosos y fallidos de otorgar privilegios </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-53 AU-2, ISO/IEC 27002:2022 5.10</t>
@@ -1327,7 +1327,7 @@
     <t xml:space="preserve">SEC-CAT-LMF-005</t>
   </si>
   <si>
-    <t xml:space="preserve">Audit successful/unsuccessful attempts to modify privileges and classifications.</t>
+    <t xml:space="preserve">La aplicación debe generar registros de auditoría para los intentos exitosos y fallidos de modificar privilegios niveles de seguridad y categorías de información </t>
   </si>
   <si>
     <t xml:space="preserve">NIST AU-2: Auditoría sobre modificaciones de privilegios. ISO/IEC 27002:2022 5.10: Registro de actividades relacionadas con control de acceso.</t>
@@ -1336,7 +1336,7 @@
     <t xml:space="preserve">SEC-CAT-LMF-006</t>
   </si>
   <si>
-    <t xml:space="preserve">Audit successful/failed privilege or object deletions.</t>
+    <t xml:space="preserve">La aplicación debe generar registros de auditoría para los intentos exitosos y fallidos de eliminación de privilegios niveles de seguridad objetos de seguridad de la base de datos y categorías de información </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-53 AU-2(3), ISO/IEC 27002:2022 5.10</t>
@@ -1348,7 +1348,7 @@
     <t xml:space="preserve">SEC-CAT-LMF-007</t>
   </si>
   <si>
-    <t xml:space="preserve">Audit privileged actions and all access attempts.</t>
+    <t xml:space="preserve">La aplicación debe generar registros de auditoría para actividades privilegiadas accesos a nivel de sistema accesos exitosos/no exitosos a objetos y todos los accesos directos al sistema de información. Se debe configurar la aplicación en los tickets de registro correspondientes a cada tipo de actividad mencionada </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-53 AU-12, ISO/IEC 27002:2022 5.10</t>
@@ -1360,7 +1360,7 @@
     <t xml:space="preserve">SEC-CAT-LMF-008</t>
   </si>
   <si>
-    <t xml:space="preserve">Log access and modification of protected data elements.</t>
+    <t xml:space="preserve">La aplicación debe registrar las acciones de los usuarios relacionadas con el acceso y los cambios de datos. Esto incluye la identificación de elementos de datos específicos que requieren protección y la auditoría de todos los accesos y modificaciones de datos </t>
   </si>
   <si>
     <t xml:space="preserve">HIPAA §164.312(b), ISO/IEC 27002:2022 5.10</t>
@@ -1372,7 +1372,7 @@
     <t xml:space="preserve">SEC-CAT-LMF-009</t>
   </si>
   <si>
-    <t xml:space="preserve">Audit privileged function executions with timestamp.</t>
+    <t xml:space="preserve">La aplicación debe auditar la ejecución de funciones privilegiadas. Configure la aplicación para registrar las entradas de registro cuando se ejecutan funciones privilegiadas. Asegúrese como mínimo de que se registre la acción específica realizada en la fecha y hora del evento </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-53 AU-12(3), ISO/IEC 27002:2022 5.10</t>
@@ -1384,7 +1384,7 @@
     <t xml:space="preserve">SEC-CAT-LMF-010</t>
   </si>
   <si>
-    <t xml:space="preserve">Log actions affecting PHI including access, update, consent, blocked data.</t>
+    <t xml:space="preserve">La aplicación debe generar registros de auditoría seguros cada vez que un usuario: 1. Acceda cree o actualice la información personal de salud (PHI) de un paciente/persona a través de la aplicación; 2. Cancele las directivas de consentimiento de un paciente/persona a través de la aplicación; 3. Acceda a través de la aplicación a datos bloqueados o enmascarados por instrucción de un paciente/persona; 4. Acceda cree o actualice los datos de registro del usuario en la aplicación </t>
   </si>
   <si>
     <t xml:space="preserve">HIPAA §164.312(b): Seguimiento de todo acceso o modificación de PHI. ISO/IEC 27002:2022 5.10: Registro de cambios sobre datos sensibles.</t>
@@ -1393,7 +1393,7 @@
     <t xml:space="preserve">SEC-CAT-LMF-011</t>
   </si>
   <si>
-    <t xml:space="preserve">Log user session start/end and session events.</t>
+    <t xml:space="preserve">La aplicación debe generar registros de auditoría que muestren el inicio y el final del acceso del usuario al sistema así como los eventos relacionados con el inicio el cierre y la duración de las sesiones </t>
   </si>
   <si>
     <t xml:space="preserve">NIST AU-12: Auditoría de sesiones. ISO/IEC 27002:2022 5.10: Registro de actividades relacionadas a inicio/cierre de sesión.</t>
@@ -1402,7 +1402,7 @@
     <t xml:space="preserve">SEC-CAT-LMF-012</t>
   </si>
   <si>
-    <t xml:space="preserve">Start logging application events at application start.</t>
+    <t xml:space="preserve">La aplicación debe iniciar la auditoría de las sesiones al inicio. Configure la aplicación para que comience a registrar los eventos de la aplicación en cuanto se inicie </t>
   </si>
   <si>
     <t xml:space="preserve">NIST AU-12: Auditoría desde el arranque de la aplicación. ISO/IEC 27002:2022 5.10: Inicio de monitoreo desde la inicialización.</t>
@@ -1411,7 +1411,7 @@
     <t xml:space="preserve">SEC-CAT-LMF-013</t>
   </si>
   <si>
-    <t xml:space="preserve">Log application closing events in event records.</t>
+    <t xml:space="preserve">La aplicación debe registrar los eventos de cierre de la aplicación. Configure la aplicación o el servidor de aplicaciones para que registre los eventos de cierre de la aplicación en los registros de eventos </t>
   </si>
   <si>
     <t xml:space="preserve">NIST AU-12: Auditoría del cierre del sistema. ISO/IEC 27002:2022 5.10: Registro de terminación de procesos.</t>
@@ -1420,7 +1420,7 @@
     <t xml:space="preserve">SEC-CAT-LMF-014</t>
   </si>
   <si>
-    <t xml:space="preserve">Generate audit records for successful/failed login attempts.</t>
+    <t xml:space="preserve">La aplicación debe generar registros de auditoría cuando se produzcan intentos de inicio de sesión ya sean exitosos o fallidos </t>
   </si>
   <si>
     <t xml:space="preserve">NIST AU-2(3): Inclusión de eventos de autenticación en registros. ISO/IEC 27002:2022 5.10: Registro de intentos de acceso exitosos y fallidos.</t>
@@ -1429,7 +1429,7 @@
     <t xml:space="preserve">SEC-CAT-LMF-015</t>
   </si>
   <si>
-    <t xml:space="preserve">Audit records must include comprehensive contextual metadata for forensic traceability.</t>
+    <t xml:space="preserve">La aplicación debe garantizar que los registros de auditoría contengan información que establezca lo siguiente: 1. Cuando se utiliza el registro centralizado; la aplicación debe incluir un identificador único para distinguirse de otros registros de aplicaciones. 2. Qué tipo de evento ocurrió; 3. La función realizada por el usuario que accede; 4. Cuándo ocurrió el evento con una marca de marca de tiempo que cumple con una granularidad de un segundo para un grado mínimo de precisión. 5. Dónde ocurrió el evento; 6. La organización del usuario que accede (al menos en aquellos casos en que una persona accede a la información en nombre de más de una organización); 7. Origen del evento que establece la identidad de cualquier persona o proceso asociado con el evento; 8. Direcciones de red y protocolos; 9. Direcciones IP de destino; 10. Identidad o ubicación del dispositivo si es posible e identificador del sistema; 11. El resultado del evento; 12. Identidad de cualquier persona sujeto u objeto/entidad asociado con el evento que utiliza el nombre de usuario o ID de usuario del usuario relacionado con el evento; 13. El rol que ejerce el usuario; 14. En caso de anulación del acceso a registros o partes de registros bloqueados o enmascarados el motivo de la anulación elegido por el usuario que accede; 15. En caso de cambios en las directivas de consentimiento realizados por un sustituto en la toma de decisiones la identidad de este. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-92: Uso de metadatos en registros para análisis forense. ISO/IEC 27002:2022 5.10: Contexto detallado en auditorías de seguridad.</t>
@@ -1438,7 +1438,7 @@
     <t xml:space="preserve">SEC-CAT-LMF-016</t>
   </si>
   <si>
-    <t xml:space="preserve">Back up audit records every 7 days to separate system.</t>
+    <t xml:space="preserve">La aplicación debe realizar copias de seguridad de los registros de auditoría al menos cada siete días en un sistema o componente diferente del auditado. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-53 AU-9(2), ISO/IEC 27002:2022 5.12</t>
@@ -1450,7 +1450,7 @@
     <t xml:space="preserve">SEC-CAT-LMF-017</t>
   </si>
   <si>
-    <t xml:space="preserve">Maintain audit records for legally mandated period (7–75 years).</t>
+    <t xml:space="preserve">La aplicación debe conservar los registros de auditoría durante un período específico, determinado por las regulaciones y estándares médicos. Esta retención debe abarcar de 7 a 75 años, según los requisitos legales y de información del Estado. Algunos estados pueden exigir que los registros médicos se conserven en el hospital para garantizar la accesibilidad continua. </t>
   </si>
   <si>
     <t xml:space="preserve">HIPAA §164.316(b)(2)(i), ISO/IEC 27002:2022 5.33</t>
@@ -1462,7 +1462,7 @@
     <t xml:space="preserve">SEC-CAT-LMF-018</t>
   </si>
   <si>
-    <t xml:space="preserve">Protect audit tools from unauthorized access or tampering.</t>
+    <t xml:space="preserve">La aplicación de gestión de registros debe garantizar el acceso y la protección contra modificaciones y eliminaciones no autorizadas, así como la integridad de las herramientas de auditoría para evitar el uso o la manipulación indebida. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-53 AU-9, ISO/IEC 27002:2022 5.12</t>
@@ -1474,7 +1474,7 @@
     <t xml:space="preserve">SEC-CAT-LMF-019</t>
   </si>
   <si>
-    <t xml:space="preserve">Control elimination, replication, and access to audit records.</t>
+    <t xml:space="preserve">La aplicación debe implementar medidas de control estrictas para la eliminación, replicación y consulta de los registros de auditoría, garantizando un control total sobre la entrada, lectura, manipulación y eliminación de datos. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST AU-9: Restricción de manipulación de auditorías. ISO/IEC 27002:2022 5.12: Control de acceso, replicación y eliminación de registros.</t>
@@ -1483,7 +1483,7 @@
     <t xml:space="preserve">SEC-CAT-LMF-020</t>
   </si>
   <si>
-    <t xml:space="preserve">Transfer audit records to a central repository.</t>
+    <t xml:space="preserve">La aplicación debe transferir registros de auditoría a un sistema o medio diferente del sistema auditado y estar configurada para escribir registros de la aplicación en un repositorio centralizado. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-92: Centralización de registros para análisis. ISO/IEC 27002:2022 5.10: Consolidación de registros de auditoría.</t>
@@ -1492,7 +1492,7 @@
     <t xml:space="preserve">SEC-CAT-LMF-021</t>
   </si>
   <si>
-    <t xml:space="preserve">Allow centralized review and filtering of audit logs.</t>
+    <t xml:space="preserve">La aplicación debe permitir la revisión y el análisis centralizado de los registros de auditoría con opciones de filtrado definidas por la organización </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-92: Análisis centralizado y correlación de eventos. ISO/IEC 27002:2022 5.10: Supervisión centralizada de registros.</t>
@@ -1501,7 +1501,7 @@
     <t xml:space="preserve">SEC-CAT-LMF-022</t>
   </si>
   <si>
-    <t xml:space="preserve">Admins must be notified automatically of updates/security alerts.</t>
+    <t xml:space="preserve">Al menos un administrador de la aplicación debe estar registrado para recibir notificaciones de actualizaciones o alertas de seguridad cuando estén disponibles automáticamente. Los administradores deben registrarse para recibir notificaciones de actualización lo que les permite detener y actualizar aplicaciones y componentes de la aplicación </t>
   </si>
   <si>
     <t xml:space="preserve">ISO/IEC 27002:2022 5.30</t>
@@ -1513,7 +1513,7 @@
     <t xml:space="preserve">SEC-CAT-LMF-023</t>
   </si>
   <si>
-    <t xml:space="preserve">Generate audit records for concurrent sessions from different workstations.</t>
+    <t xml:space="preserve">La aplicación debe generar registros de auditoría cuando se produce una sesión simultánea desde diferentes estaciones de trabajo </t>
   </si>
   <si>
     <t xml:space="preserve">NIST AU-2(3): Registro detallado de sesiones simultáneas. ISO/IEC 27002:2022 5.10: Auditoría de sesiones concurrentes y su trazabilidad.</t>
@@ -1522,7 +1522,7 @@
     <t xml:space="preserve">SEC-CAT-LMF-024</t>
   </si>
   <si>
-    <t xml:space="preserve">EHRI must track and report access to patient records with detailed user and event tracing.</t>
+    <t xml:space="preserve">El EHRI debe poder registrar e informar de forma segura cada acceso a los registros de un paciente/persona, cumpliendo con los siguientes requisitos: 1. Identificar a todos los usuarios que han accedido o modificado los registros de un paciente/persona en un período determinado. 2. Proporcionar funcionalidad para informar a un usuario determinado: • Los registros a los que puede acceder. • Puede acceder a las secciones específicas del/de los registro(s). • Los privilegios que tiene sobre cada uno de estos registros. 3. Identificar a todos los pacientes/personas cuyos registros han sido accedidos o modificados por un usuario específico en un período determinado. 4. El sistema debe generar un evento de seguridad en caso de un intento o posible éxito de violar los controles de inicio de sesión. </t>
   </si>
   <si>
     <t xml:space="preserve">HIPAA §164.312(b): Registros de auditoría que monitorean accesos a ePHI. ISO/IEC 27002:2022 5.10: Seguimiento de accesos a información sensible.</t>
@@ -1531,7 +1531,7 @@
     <t xml:space="preserve">SEC-CAT-LMF-025</t>
   </si>
   <si>
-    <t xml:space="preserve">Notify admin and audit configuration changes.</t>
+    <t xml:space="preserve">La aplicación debe notificar al administrador, auditar y registrar las modificaciones realizadas en la configuración de la aplicación. </t>
   </si>
   <si>
     <t xml:space="preserve">NIST AU-12(3): Notificaciones de cambios de configuración auditables. ISO/IEC 27002:2022 5.10: Registro y alerta de cambios relevantes.</t>
@@ -1540,7 +1540,7 @@
     <t xml:space="preserve">SEC-CAT-LMF-026</t>
   </si>
   <si>
-    <t xml:space="preserve">Notify admin and ISSO of account activation.</t>
+    <t xml:space="preserve">La aplicación debe notificar a los administradores del sistema y a los responsables de seguridad del sistema (ISSO) sobre las acciones de activación de cuentas. La aplicación debe estar configurada para enviar notificaciones al administrador del sistema y al ISSO cuando se habilitan las cuentas de la aplicación </t>
   </si>
   <si>
     <t xml:space="preserve">ISO/IEC 27002:2022 5.18</t>
@@ -1552,7 +1552,7 @@
     <t xml:space="preserve">SEC-CAT-LMF-027</t>
   </si>
   <si>
-    <t xml:space="preserve">Notify admin and ISSO of account deactivation.</t>
+    <t xml:space="preserve">La aplicación debe notificar a los administradores del sistema y a los responsables de seguridad del sistema (ISSO) sobre las acciones de desactivación de cuentas. La aplicación debe estar configurada para enviar notificaciones al administrador del sistema y al ISSO cuando se habilitan las cuentas de la aplicación </t>
   </si>
   <si>
     <t xml:space="preserve">ISO/IEC 27002:2022 5.18: Gestión del ciclo de vida de cuentas incluyendo notificaciones de desactivación.</t>
@@ -1561,7 +1561,7 @@
     <t xml:space="preserve">SEC-CAT-LMF-028</t>
   </si>
   <si>
-    <t xml:space="preserve">Notify admin and ISSO when accounts are created.</t>
+    <t xml:space="preserve">La aplicación debe notificar a los administradores del sistema y a los responsables de seguridad del sistema (ISSO) sobre la creación de cuentas de la aplicación </t>
   </si>
   <si>
     <t xml:space="preserve">ISO/IEC 27002:2022 5.18: Notificación de creación de cuentas como medida de control de acceso.</t>
@@ -1570,7 +1570,7 @@
     <t xml:space="preserve">SEC-CAT-LMF-029</t>
   </si>
   <si>
-    <t xml:space="preserve">Notify admin and ISSO of account deletions.</t>
+    <t xml:space="preserve">La aplicación debe notificar a los administradores del sistema y a los responsables de seguridad de la información del sistema (ISSO) sobre las acciones de eliminación de cuentas. La configuración de la aplicación debe incluir la notificación al administrador del sistema y al ISSO cuando se eliminan las cuentas de la aplicación </t>
   </si>
   <si>
     <t xml:space="preserve">ISO/IEC 27002:2022 5.18: Seguimiento de eventos de eliminación de cuentas con alertas correspondientes.</t>
@@ -1579,7 +1579,7 @@
     <t xml:space="preserve">SEC-CAT-LMF-030</t>
   </si>
   <si>
-    <t xml:space="preserve">Notify admin and ISSO of account modifications.</t>
+    <t xml:space="preserve">La aplicación debe notificar a los administradores del sistema y a los oficiales de seguridad del sistema (ISSO) cuando se modifican las cuentas de usuario </t>
   </si>
   <si>
     <t xml:space="preserve">ISO/IEC 27002:2022 5.18: Notificación sobre cambios en atributos de cuentas.</t>
@@ -1588,7 +1588,7 @@
     <t xml:space="preserve">SEC-CAT-LMF-031</t>
   </si>
   <si>
-    <t xml:space="preserve">Analyze audit logs to identify users accessing/modifying patient records.</t>
+    <t xml:space="preserve">La aplicación debe proporcionar funciones para analizar registros y auditar rastros a fin de identificar a todos los usuarios que han accedido o modificado registros de pacientes/personas durante un período determinado </t>
   </si>
   <si>
     <t xml:space="preserve">HIPAA §164.312(b): Análisis de auditoría para detectar accesos a ePHI. ISO/IEC 27002:2022 5.10: Correlación de eventos de acceso.</t>
@@ -1597,7 +1597,7 @@
     <t xml:space="preserve">SEC-CAT-LMF-032</t>
   </si>
   <si>
-    <t xml:space="preserve">Alert ISSO and SA on audit processing failure.</t>
+    <t xml:space="preserve">La aplicación debe alertar al Oficial de Seguridad de la Información (ISSO) y al Administrador del Sistema (SA) en caso de una falla en el procesamiento de la auditoría. La aplicación debe estar configurada para enviar una alarma cuando el sistema de auditoría falla o está experimentando una falla </t>
   </si>
   <si>
     <t xml:space="preserve">NIST SP 800-53 AU-5, ISO/IEC 27002:2022 5.10</t>
@@ -1609,7 +1609,7 @@
     <t xml:space="preserve">SEC-CAT-SRF-001</t>
   </si>
   <si>
-    <t xml:space="preserve">Protect against SSRF with network and application controls.</t>
+    <t xml:space="preserve">La aplicación debe implementar medidas de protección para prevenir vulnerabilidades de SSRF incluyendo controles de red y de capa de aplicación </t>
   </si>
   <si>
     <t xml:space="preserve">OWASP Top 10 2021 A10, CWE-918</t>
@@ -1713,16 +1713,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1920,2413 +1924,2413 @@
   </sheetPr>
   <dimension ref="A1:E141"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A97" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A143" activeCellId="0" sqref="A143"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A89" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B144" activeCellId="0" sqref="B144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="121.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="73.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="289.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="121.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="73.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="289.15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="D4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="D5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="D6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="D7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="2" t="s">
+      <c r="D8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="2" t="s">
+      <c r="D9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="2" t="s">
+      <c r="D10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="2" t="s">
+      <c r="D11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="2" t="s">
+      <c r="D12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="2" t="s">
+      <c r="D13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="2" t="s">
+      <c r="D14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="2" t="s">
+      <c r="D15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="2" t="s">
+      <c r="D16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="2" t="s">
+      <c r="D17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="2" t="s">
+      <c r="D18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="2" t="s">
+      <c r="D19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="2" t="s">
+      <c r="D20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="2" t="s">
+      <c r="D21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="2" t="s">
+      <c r="D22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="2" t="s">
+      <c r="D23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" s="2" t="s">
+      <c r="D24" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="2" t="s">
+      <c r="D25" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" s="2" t="s">
+      <c r="D26" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" s="2" t="s">
+      <c r="D27" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E28" s="2" t="s">
+      <c r="D28" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="3" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29" s="2" t="s">
+      <c r="D29" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" s="2" t="s">
+      <c r="D30" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="3" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" s="2" t="s">
+      <c r="D31" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32" s="2" t="s">
+      <c r="D32" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="3" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E33" s="2" t="s">
+      <c r="D33" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="3" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E34" s="2" t="s">
+      <c r="D34" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="3" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E35" s="2" t="s">
+      <c r="D35" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="3" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E36" s="2" t="s">
+      <c r="D36" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="3" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E37" s="2" t="s">
+      <c r="D37" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" s="2" t="s">
+      <c r="D38" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E39" s="2" t="s">
+      <c r="D39" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="3" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E40" s="2" t="s">
+      <c r="D40" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="3" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E41" s="2" t="s">
+      <c r="D41" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="3" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E42" s="2" t="s">
+      <c r="D42" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="3" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E43" s="2" t="s">
+      <c r="D43" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="3" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E44" s="2" t="s">
+      <c r="D44" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="3" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E45" s="2" t="s">
+      <c r="D45" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="3" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="D46" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E46" s="2" t="s">
+      <c r="D46" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="3" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="D47" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E47" s="2" t="s">
+      <c r="D47" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" s="3" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D48" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E48" s="2" t="s">
+      <c r="D48" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="3" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C49" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="D49" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E49" s="2" t="s">
+      <c r="D49" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" s="3" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C50" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E50" s="2" t="s">
+      <c r="D50" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" s="3" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C51" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E51" s="2" t="s">
+      <c r="D51" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51" s="3" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C52" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E52" s="2" t="s">
+      <c r="D52" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E52" s="3" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="2" t="s">
+      <c r="A53" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C53" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E53" s="2" t="s">
+      <c r="D53" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" s="3" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="2" t="s">
+      <c r="A54" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B54" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C54" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="D54" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E54" s="2" t="s">
+      <c r="D54" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E54" s="3" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="2" t="s">
+      <c r="A55" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B55" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C55" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="D55" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E55" s="2" t="s">
+      <c r="D55" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E55" s="3" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="2" t="s">
+      <c r="A56" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C56" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="D56" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E56" s="2" t="s">
+      <c r="D56" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E56" s="3" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="2" t="s">
+      <c r="A57" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C57" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="D57" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E57" s="2" t="s">
+      <c r="D57" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E57" s="3" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="2" t="s">
+      <c r="A58" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B58" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C58" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="D58" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E58" s="2" t="s">
+      <c r="D58" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" s="3" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="2" t="s">
+      <c r="A59" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B59" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C59" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="D59" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E59" s="2" t="s">
+      <c r="D59" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" s="3" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="2" t="s">
+      <c r="A60" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B60" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C60" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="D60" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E60" s="2" t="s">
+      <c r="D60" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E60" s="3" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="2" t="s">
+      <c r="A61" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B61" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C61" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="D61" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E61" s="2" t="s">
+      <c r="D61" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" s="3" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="2" t="s">
+      <c r="A62" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B62" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C62" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="D62" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E62" s="2" t="s">
+      <c r="D62" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62" s="3" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="2" t="s">
+      <c r="A63" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B63" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C63" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="D63" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E63" s="2" t="s">
+      <c r="D63" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E63" s="3" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="2" t="s">
+      <c r="A64" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B64" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C64" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="D64" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E64" s="2" t="s">
+      <c r="D64" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E64" s="3" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="2" t="s">
+      <c r="A65" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B65" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C65" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="D65" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E65" s="2" t="s">
+      <c r="D65" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E65" s="3" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="2" t="s">
+      <c r="A66" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B66" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C66" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="D66" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E66" s="2" t="s">
+      <c r="D66" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E66" s="3" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="2" t="s">
+      <c r="A67" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B67" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C67" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="D67" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E67" s="2" t="s">
+      <c r="D67" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E67" s="3" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="2" t="s">
+      <c r="A68" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B68" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C68" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="D68" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E68" s="2" t="s">
+      <c r="D68" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E68" s="3" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="2" t="s">
+      <c r="A69" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B69" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="C69" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="D69" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E69" s="2" t="s">
+      <c r="D69" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E69" s="3" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="2" t="s">
+      <c r="A70" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B70" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="C70" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="D70" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E70" s="2" t="s">
+      <c r="D70" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E70" s="3" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="2" t="s">
+      <c r="A71" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B71" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C71" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="D71" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E71" s="2" t="s">
+      <c r="D71" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E71" s="3" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="2" t="s">
+      <c r="A72" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B72" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="C72" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="D72" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E72" s="2" t="s">
+      <c r="D72" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E72" s="3" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="2" t="s">
+      <c r="A73" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B73" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="C73" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="D73" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E73" s="2" t="s">
+      <c r="D73" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E73" s="3" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="2" t="s">
+      <c r="A74" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B74" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="C74" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="D74" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E74" s="2" t="s">
+      <c r="D74" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E74" s="3" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="2" t="s">
+      <c r="A75" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B75" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C75" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="D75" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E75" s="2" t="s">
+      <c r="D75" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E75" s="3" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="2" t="s">
+      <c r="A76" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B76" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C76" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="D76" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E76" s="2" t="s">
+      <c r="D76" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E76" s="3" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="2" t="s">
+      <c r="A77" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B77" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="C77" s="2" t="s">
+      <c r="C77" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="D77" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E77" s="2" t="s">
+      <c r="D77" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E77" s="3" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="2" t="s">
+      <c r="A78" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B78" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="C78" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="D78" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E78" s="2" t="s">
+      <c r="D78" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E78" s="3" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="2" t="s">
+      <c r="A79" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B79" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="C79" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="D79" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E79" s="2" t="s">
+      <c r="D79" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E79" s="3" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="2" t="s">
+      <c r="A80" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B80" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="C80" s="2" t="s">
+      <c r="C80" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="D80" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E80" s="2" t="s">
+      <c r="D80" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E80" s="3" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="2" t="s">
+      <c r="A81" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B81" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="C81" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="D81" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E81" s="2" t="s">
+      <c r="D81" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E81" s="3" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="2" t="s">
+      <c r="A82" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B82" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="C82" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="D82" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E82" s="2" t="s">
+      <c r="D82" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E82" s="3" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="2" t="s">
+      <c r="A83" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B83" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="C83" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="D83" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E83" s="2" t="s">
+      <c r="D83" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E83" s="3" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="2" t="s">
+      <c r="A84" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B84" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="C84" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="D84" s="2" t="s">
+      <c r="D84" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="E84" s="2" t="s">
+      <c r="E84" s="3" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="2" t="s">
+      <c r="A85" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="B85" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="C85" s="2" t="s">
+      <c r="C85" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="D85" s="2" t="s">
+      <c r="D85" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="E85" s="2" t="s">
+      <c r="E85" s="3" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="2" t="s">
+      <c r="A86" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B86" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="C86" s="2" t="s">
+      <c r="C86" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="D86" s="2" t="s">
+      <c r="D86" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="E86" s="2" t="s">
+      <c r="E86" s="3" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="2" t="s">
+      <c r="A87" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="B87" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="C87" s="2" t="s">
+      <c r="C87" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="D87" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E87" s="2" t="s">
+      <c r="D87" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E87" s="3" t="s">
         <v>342</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="2" t="s">
+      <c r="A88" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="B88" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="C88" s="2" t="s">
+      <c r="C88" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="D88" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E88" s="2" t="s">
+      <c r="D88" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E88" s="3" t="s">
         <v>346</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="2" t="s">
+      <c r="A89" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B89" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="C89" s="2" t="s">
+      <c r="C89" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="D89" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E89" s="2" t="s">
+      <c r="D89" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E89" s="3" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="2" t="s">
+      <c r="A90" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="B90" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="C90" s="2" t="s">
+      <c r="C90" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="D90" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E90" s="2" t="s">
+      <c r="D90" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E90" s="3" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="2" t="s">
+      <c r="A91" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="B91" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="C91" s="2" t="s">
+      <c r="C91" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="D91" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E91" s="2" t="s">
+      <c r="D91" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E91" s="3" t="s">
         <v>356</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="2" t="s">
+      <c r="A92" s="3" t="s">
         <v>357</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="B92" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="C92" s="2" t="s">
+      <c r="C92" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="D92" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E92" s="2" t="s">
+      <c r="D92" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E92" s="3" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="2" t="s">
+      <c r="A93" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="B93" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="C93" s="2" t="s">
+      <c r="C93" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="D93" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E93" s="2" t="s">
+      <c r="D93" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E93" s="3" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="2" t="s">
+      <c r="A94" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="B94" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="C94" s="2" t="s">
+      <c r="C94" s="3" t="s">
         <v>367</v>
       </c>
-      <c r="D94" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E94" s="2" t="s">
+      <c r="D94" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E94" s="3" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="2" t="s">
+      <c r="A95" s="3" t="s">
         <v>369</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="B95" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="C95" s="2" t="s">
+      <c r="C95" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="D95" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E95" s="2" t="s">
+      <c r="D95" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E95" s="3" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="2" t="s">
+      <c r="A96" s="3" t="s">
         <v>372</v>
       </c>
-      <c r="B96" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="C96" s="2" t="s">
+      <c r="B96" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="C96" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="D96" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E96" s="2" t="s">
-        <v>373</v>
+      <c r="D96" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="B97" s="2" t="s">
+      <c r="A97" s="3" t="s">
         <v>375</v>
       </c>
-      <c r="C97" s="2" t="s">
+      <c r="B97" s="3" t="s">
         <v>376</v>
       </c>
-      <c r="D97" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E97" s="2" t="s">
+      <c r="C97" s="3" t="s">
         <v>377</v>
       </c>
+      <c r="D97" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>378</v>
+      </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="B98" s="2" t="s">
+      <c r="A98" s="3" t="s">
         <v>379</v>
       </c>
-      <c r="C98" s="2" t="s">
+      <c r="B98" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="D98" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E98" s="2" t="s">
+      <c r="C98" s="3" t="s">
         <v>381</v>
       </c>
+      <c r="D98" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E98" s="3" t="s">
+        <v>382</v>
+      </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="B99" s="2" t="s">
+      <c r="A99" s="3" t="s">
         <v>383</v>
       </c>
-      <c r="C99" s="2" t="s">
+      <c r="B99" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="D99" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E99" s="2" t="s">
+      <c r="C99" s="3" t="s">
         <v>385</v>
       </c>
+      <c r="D99" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>386</v>
+      </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="B100" s="2" t="s">
+      <c r="A100" s="3" t="s">
         <v>387</v>
       </c>
-      <c r="C100" s="2" t="s">
+      <c r="B100" s="3" t="s">
         <v>388</v>
       </c>
-      <c r="D100" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E100" s="2" t="s">
+      <c r="C100" s="3" t="s">
         <v>389</v>
       </c>
+      <c r="D100" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E100" s="3" t="s">
+        <v>390</v>
+      </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="B101" s="2" t="s">
+      <c r="A101" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="C101" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="D101" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E101" s="2" t="s">
+      <c r="B101" s="3" t="s">
         <v>392</v>
       </c>
+      <c r="C101" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E101" s="3" t="s">
+        <v>393</v>
+      </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="B102" s="2" t="s">
+      <c r="A102" s="3" t="s">
         <v>394</v>
       </c>
-      <c r="C102" s="2" t="s">
+      <c r="B102" s="3" t="s">
         <v>395</v>
       </c>
-      <c r="D102" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E102" s="2" t="s">
+      <c r="C102" s="3" t="s">
         <v>396</v>
       </c>
+      <c r="D102" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>397</v>
+      </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="B103" s="2" t="s">
+      <c r="A103" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="C103" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="D103" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E103" s="2" t="s">
+      <c r="B103" s="3" t="s">
         <v>399</v>
       </c>
+      <c r="C103" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E103" s="3" t="s">
+        <v>400</v>
+      </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="B104" s="2" t="s">
+      <c r="A104" s="3" t="s">
         <v>401</v>
       </c>
-      <c r="C104" s="2" t="s">
+      <c r="B104" s="3" t="s">
         <v>402</v>
       </c>
-      <c r="D104" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E104" s="2" t="s">
+      <c r="C104" s="3" t="s">
         <v>403</v>
       </c>
+      <c r="D104" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E104" s="3" t="s">
+        <v>404</v>
+      </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="2" t="s">
-        <v>404</v>
-      </c>
-      <c r="B105" s="2" t="s">
+      <c r="A105" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="C105" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="D105" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E105" s="2" t="s">
+      <c r="B105" s="3" t="s">
         <v>406</v>
       </c>
+      <c r="C105" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E105" s="3" t="s">
+        <v>407</v>
+      </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="2" t="s">
-        <v>407</v>
-      </c>
-      <c r="B106" s="2" t="s">
+      <c r="A106" s="3" t="s">
         <v>408</v>
       </c>
-      <c r="C106" s="2" t="s">
+      <c r="B106" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="D106" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E106" s="2" t="s">
+      <c r="C106" s="3" t="s">
         <v>410</v>
       </c>
+      <c r="D106" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E106" s="3" t="s">
+        <v>411</v>
+      </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="2" t="s">
-        <v>411</v>
-      </c>
-      <c r="B107" s="2" t="s">
+      <c r="A107" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="C107" s="2" t="s">
+      <c r="B107" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="D107" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E107" s="2" t="s">
+      <c r="C107" s="3" t="s">
         <v>414</v>
       </c>
+      <c r="D107" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E107" s="3" t="s">
+        <v>415</v>
+      </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="B108" s="2" t="s">
+      <c r="A108" s="3" t="s">
         <v>416</v>
       </c>
-      <c r="C108" s="2" t="s">
+      <c r="B108" s="3" t="s">
         <v>417</v>
       </c>
-      <c r="D108" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E108" s="2" t="s">
+      <c r="C108" s="3" t="s">
         <v>418</v>
       </c>
+      <c r="D108" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E108" s="3" t="s">
+        <v>419</v>
+      </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="B109" s="2" t="s">
+      <c r="A109" s="3" t="s">
         <v>420</v>
       </c>
-      <c r="C109" s="2" t="s">
+      <c r="B109" s="3" t="s">
         <v>421</v>
       </c>
-      <c r="D109" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E109" s="2" t="s">
+      <c r="C109" s="3" t="s">
         <v>422</v>
       </c>
+      <c r="D109" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E109" s="3" t="s">
+        <v>423</v>
+      </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="B110" s="2" t="s">
+      <c r="A110" s="3" t="s">
         <v>424</v>
       </c>
-      <c r="C110" s="2" t="s">
+      <c r="B110" s="3" t="s">
         <v>421</v>
       </c>
-      <c r="D110" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E110" s="2" t="s">
+      <c r="C110" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E110" s="3" t="s">
         <v>425</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="2" t="s">
+      <c r="A111" s="3" t="s">
         <v>426</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="B111" s="3" t="s">
         <v>427</v>
       </c>
-      <c r="C111" s="2" t="s">
+      <c r="C111" s="3" t="s">
         <v>428</v>
       </c>
-      <c r="D111" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E111" s="2" t="s">
+      <c r="D111" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E111" s="3" t="s">
         <v>429</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="2" t="s">
+      <c r="A112" s="3" t="s">
         <v>430</v>
       </c>
-      <c r="B112" s="2" t="s">
+      <c r="B112" s="3" t="s">
         <v>431</v>
       </c>
-      <c r="C112" s="2" t="s">
+      <c r="C112" s="3" t="s">
         <v>432</v>
       </c>
-      <c r="D112" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E112" s="2" t="s">
+      <c r="D112" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E112" s="3" t="s">
         <v>433</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="2" t="s">
+      <c r="A113" s="3" t="s">
         <v>434</v>
       </c>
-      <c r="B113" s="2" t="s">
+      <c r="B113" s="3" t="s">
         <v>435</v>
       </c>
-      <c r="C113" s="2" t="s">
+      <c r="C113" s="3" t="s">
         <v>432</v>
       </c>
-      <c r="D113" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E113" s="2" t="s">
+      <c r="D113" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E113" s="3" t="s">
         <v>436</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="2" t="s">
+      <c r="A114" s="3" t="s">
         <v>437</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="B114" s="3" t="s">
         <v>438</v>
       </c>
-      <c r="C114" s="2" t="s">
+      <c r="C114" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="D114" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E114" s="2" t="s">
+      <c r="D114" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E114" s="3" t="s">
         <v>440</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="2" t="s">
+      <c r="A115" s="3" t="s">
         <v>441</v>
       </c>
-      <c r="B115" s="2" t="s">
+      <c r="B115" s="3" t="s">
         <v>442</v>
       </c>
-      <c r="C115" s="2" t="s">
+      <c r="C115" s="3" t="s">
         <v>443</v>
       </c>
-      <c r="D115" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E115" s="2" t="s">
+      <c r="D115" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E115" s="3" t="s">
         <v>444</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="2" t="s">
+      <c r="A116" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="B116" s="3" t="s">
         <v>446</v>
       </c>
-      <c r="C116" s="2" t="s">
+      <c r="C116" s="3" t="s">
         <v>447</v>
       </c>
-      <c r="D116" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E116" s="2" t="s">
+      <c r="D116" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E116" s="3" t="s">
         <v>448</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="2" t="s">
+      <c r="A117" s="3" t="s">
         <v>449</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="B117" s="3" t="s">
         <v>450</v>
       </c>
-      <c r="C117" s="2" t="s">
+      <c r="C117" s="3" t="s">
         <v>451</v>
       </c>
-      <c r="D117" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E117" s="2" t="s">
+      <c r="D117" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E117" s="3" t="s">
         <v>452</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="2" t="s">
+      <c r="A118" s="3" t="s">
         <v>453</v>
       </c>
-      <c r="B118" s="2" t="s">
+      <c r="B118" s="3" t="s">
         <v>454</v>
       </c>
-      <c r="C118" s="2" t="s">
+      <c r="C118" s="3" t="s">
         <v>447</v>
       </c>
-      <c r="D118" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E118" s="2" t="s">
+      <c r="D118" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E118" s="3" t="s">
         <v>455</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="2" t="s">
+      <c r="A119" s="3" t="s">
         <v>456</v>
       </c>
-      <c r="B119" s="2" t="s">
+      <c r="B119" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="C119" s="2" t="s">
+      <c r="C119" s="3" t="s">
         <v>443</v>
       </c>
-      <c r="D119" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E119" s="2" t="s">
+      <c r="D119" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E119" s="3" t="s">
         <v>458</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="2" t="s">
+      <c r="A120" s="3" t="s">
         <v>459</v>
       </c>
-      <c r="B120" s="2" t="s">
+      <c r="B120" s="3" t="s">
         <v>460</v>
       </c>
-      <c r="C120" s="2" t="s">
+      <c r="C120" s="3" t="s">
         <v>443</v>
       </c>
-      <c r="D120" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E120" s="2" t="s">
+      <c r="D120" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E120" s="3" t="s">
         <v>461</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="2" t="s">
+      <c r="A121" s="3" t="s">
         <v>462</v>
       </c>
-      <c r="B121" s="2" t="s">
+      <c r="B121" s="3" t="s">
         <v>463</v>
       </c>
-      <c r="C121" s="2" t="s">
+      <c r="C121" s="3" t="s">
         <v>443</v>
       </c>
-      <c r="D121" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E121" s="2" t="s">
+      <c r="D121" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E121" s="3" t="s">
         <v>464</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="2" t="s">
+      <c r="A122" s="3" t="s">
         <v>465</v>
       </c>
-      <c r="B122" s="2" t="s">
+      <c r="B122" s="3" t="s">
         <v>466</v>
       </c>
-      <c r="C122" s="2" t="s">
+      <c r="C122" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="D122" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E122" s="2" t="s">
+      <c r="D122" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E122" s="3" t="s">
         <v>467</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="2" t="s">
+      <c r="A123" s="3" t="s">
         <v>468</v>
       </c>
-      <c r="B123" s="2" t="s">
+      <c r="B123" s="3" t="s">
         <v>469</v>
       </c>
-      <c r="C123" s="2" t="s">
+      <c r="C123" s="3" t="s">
         <v>428</v>
       </c>
-      <c r="D123" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E123" s="2" t="s">
+      <c r="D123" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E123" s="3" t="s">
         <v>470</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="2" t="s">
+      <c r="A124" s="3" t="s">
         <v>471</v>
       </c>
-      <c r="B124" s="2" t="s">
+      <c r="B124" s="3" t="s">
         <v>472</v>
       </c>
-      <c r="C124" s="2" t="s">
+      <c r="C124" s="3" t="s">
         <v>473</v>
       </c>
-      <c r="D124" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E124" s="2" t="s">
+      <c r="D124" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E124" s="3" t="s">
         <v>474</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="2" t="s">
+      <c r="A125" s="3" t="s">
         <v>475</v>
       </c>
-      <c r="B125" s="2" t="s">
+      <c r="B125" s="3" t="s">
         <v>476</v>
       </c>
-      <c r="C125" s="2" t="s">
+      <c r="C125" s="3" t="s">
         <v>477</v>
       </c>
-      <c r="D125" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E125" s="2" t="s">
+      <c r="D125" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E125" s="3" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="2" t="s">
+      <c r="A126" s="3" t="s">
         <v>479</v>
       </c>
-      <c r="B126" s="2" t="s">
+      <c r="B126" s="3" t="s">
         <v>480</v>
       </c>
-      <c r="C126" s="2" t="s">
+      <c r="C126" s="3" t="s">
         <v>481</v>
       </c>
-      <c r="D126" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E126" s="2" t="s">
+      <c r="D126" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E126" s="3" t="s">
         <v>482</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="2" t="s">
+      <c r="A127" s="3" t="s">
         <v>483</v>
       </c>
-      <c r="B127" s="2" t="s">
+      <c r="B127" s="3" t="s">
         <v>484</v>
       </c>
-      <c r="C127" s="2" t="s">
+      <c r="C127" s="3" t="s">
         <v>481</v>
       </c>
-      <c r="D127" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E127" s="2" t="s">
+      <c r="D127" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E127" s="3" t="s">
         <v>485</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="2" t="s">
+      <c r="A128" s="3" t="s">
         <v>486</v>
       </c>
-      <c r="B128" s="2" t="s">
+      <c r="B128" s="3" t="s">
         <v>487</v>
       </c>
-      <c r="C128" s="2" t="s">
+      <c r="C128" s="3" t="s">
         <v>428</v>
       </c>
-      <c r="D128" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E128" s="2" t="s">
+      <c r="D128" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E128" s="3" t="s">
         <v>488</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="2" t="s">
+      <c r="A129" s="3" t="s">
         <v>489</v>
       </c>
-      <c r="B129" s="2" t="s">
+      <c r="B129" s="3" t="s">
         <v>490</v>
       </c>
-      <c r="C129" s="2" t="s">
+      <c r="C129" s="3" t="s">
         <v>428</v>
       </c>
-      <c r="D129" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E129" s="2" t="s">
+      <c r="D129" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E129" s="3" t="s">
         <v>491</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="2" t="s">
+      <c r="A130" s="3" t="s">
         <v>492</v>
       </c>
-      <c r="B130" s="2" t="s">
+      <c r="B130" s="3" t="s">
         <v>493</v>
       </c>
-      <c r="C130" s="2" t="s">
+      <c r="C130" s="3" t="s">
         <v>494</v>
       </c>
-      <c r="D130" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E130" s="2" t="s">
+      <c r="D130" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E130" s="3" t="s">
         <v>495</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="2" t="s">
+      <c r="A131" s="3" t="s">
         <v>496</v>
       </c>
-      <c r="B131" s="2" t="s">
+      <c r="B131" s="3" t="s">
         <v>497</v>
       </c>
-      <c r="C131" s="2" t="s">
+      <c r="C131" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="D131" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E131" s="2" t="s">
+      <c r="D131" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E131" s="3" t="s">
         <v>498</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="2" t="s">
+      <c r="A132" s="3" t="s">
         <v>499</v>
       </c>
-      <c r="B132" s="2" t="s">
+      <c r="B132" s="3" t="s">
         <v>500</v>
       </c>
-      <c r="C132" s="2" t="s">
+      <c r="C132" s="3" t="s">
         <v>447</v>
       </c>
-      <c r="D132" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E132" s="2" t="s">
+      <c r="D132" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E132" s="3" t="s">
         <v>501</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="2" t="s">
+      <c r="A133" s="3" t="s">
         <v>502</v>
       </c>
-      <c r="B133" s="2" t="s">
+      <c r="B133" s="3" t="s">
         <v>503</v>
       </c>
-      <c r="C133" s="2" t="s">
+      <c r="C133" s="3" t="s">
         <v>451</v>
       </c>
-      <c r="D133" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E133" s="2" t="s">
+      <c r="D133" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E133" s="3" t="s">
         <v>504</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="2" t="s">
+      <c r="A134" s="3" t="s">
         <v>505</v>
       </c>
-      <c r="B134" s="2" t="s">
+      <c r="B134" s="3" t="s">
         <v>506</v>
       </c>
-      <c r="C134" s="2" t="s">
+      <c r="C134" s="3" t="s">
         <v>507</v>
       </c>
-      <c r="D134" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E134" s="2" t="s">
+      <c r="D134" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E134" s="3" t="s">
         <v>508</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="2" t="s">
+      <c r="A135" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="B135" s="2" t="s">
+      <c r="B135" s="3" t="s">
         <v>510</v>
       </c>
-      <c r="C135" s="2" t="s">
+      <c r="C135" s="3" t="s">
         <v>507</v>
       </c>
-      <c r="D135" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E135" s="2" t="s">
+      <c r="D135" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E135" s="3" t="s">
         <v>511</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="2" t="s">
+      <c r="A136" s="3" t="s">
         <v>512</v>
       </c>
-      <c r="B136" s="2" t="s">
+      <c r="B136" s="3" t="s">
         <v>513</v>
       </c>
-      <c r="C136" s="2" t="s">
+      <c r="C136" s="3" t="s">
         <v>507</v>
       </c>
-      <c r="D136" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E136" s="2" t="s">
+      <c r="D136" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E136" s="3" t="s">
         <v>514</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="2" t="s">
+      <c r="A137" s="3" t="s">
         <v>515</v>
       </c>
-      <c r="B137" s="2" t="s">
+      <c r="B137" s="3" t="s">
         <v>516</v>
       </c>
-      <c r="C137" s="2" t="s">
+      <c r="C137" s="3" t="s">
         <v>507</v>
       </c>
-      <c r="D137" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E137" s="2" t="s">
+      <c r="D137" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E137" s="3" t="s">
         <v>517</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="2" t="s">
+      <c r="A138" s="3" t="s">
         <v>518</v>
       </c>
-      <c r="B138" s="2" t="s">
+      <c r="B138" s="3" t="s">
         <v>519</v>
       </c>
-      <c r="C138" s="2" t="s">
+      <c r="C138" s="3" t="s">
         <v>507</v>
       </c>
-      <c r="D138" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E138" s="2" t="s">
+      <c r="D138" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E138" s="3" t="s">
         <v>520</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="2" t="s">
+      <c r="A139" s="3" t="s">
         <v>521</v>
       </c>
-      <c r="B139" s="2" t="s">
+      <c r="B139" s="3" t="s">
         <v>522</v>
       </c>
-      <c r="C139" s="2" t="s">
+      <c r="C139" s="3" t="s">
         <v>447</v>
       </c>
-      <c r="D139" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E139" s="2" t="s">
+      <c r="D139" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E139" s="3" t="s">
         <v>523</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="2" t="s">
+      <c r="A140" s="3" t="s">
         <v>524</v>
       </c>
-      <c r="B140" s="2" t="s">
+      <c r="B140" s="3" t="s">
         <v>525</v>
       </c>
-      <c r="C140" s="2" t="s">
+      <c r="C140" s="3" t="s">
         <v>526</v>
       </c>
-      <c r="D140" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E140" s="2" t="s">
+      <c r="D140" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E140" s="3" t="s">
         <v>527</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="2" t="s">
+      <c r="A141" s="3" t="s">
         <v>528</v>
       </c>
-      <c r="B141" s="2" t="s">
+      <c r="B141" s="3" t="s">
         <v>529</v>
       </c>
-      <c r="C141" s="2" t="s">
+      <c r="C141" s="3" t="s">
         <v>530</v>
       </c>
-      <c r="D141" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E141" s="2" t="s">
+      <c r="D141" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E141" s="3" t="s">
         <v>531</v>
       </c>
     </row>

</xml_diff>